<commit_message>
add scrape data ipynb
</commit_message>
<xml_diff>
--- a/etc/flask_web_chart.xlsx
+++ b/etc/flask_web_chart.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView windowWidth="22368" windowHeight="9215"/>
+    <workbookView windowWidth="22368" windowHeight="9215" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectSchedule" sheetId="11" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="69">
   <si>
     <t>Create a Project Schedule in this worksheet.
 Enter title of this project in cell B1. 
@@ -162,7 +162,13 @@
     <t>Sample phase title block</t>
   </si>
   <si>
-    <t>Phase 3 Title</t>
+    <t>Sprint 2</t>
+  </si>
+  <si>
+    <t>cleaning</t>
+  </si>
+  <si>
+    <t>django</t>
   </si>
   <si>
     <t>Phase 4 Title</t>
@@ -220,22 +226,13 @@
     <t>Able to display popular attractions from destination</t>
   </si>
   <si>
-    <t>website skeleton</t>
-  </si>
-  <si>
     <t>Allows customization and self drag and plan of attractions</t>
   </si>
   <si>
     <t>Scraper</t>
   </si>
   <si>
-    <t>database/framework</t>
-  </si>
-  <si>
     <t>Details on the attractions (e.g location,distance)</t>
-  </si>
-  <si>
-    <t>model</t>
   </si>
   <si>
     <t>Shortest path suggestiong -&gt; A *</t>
@@ -276,15 +273,15 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="9">
-    <numFmt numFmtId="176" formatCode="ddd\,\ m/d/yyyy"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="d"/>
-    <numFmt numFmtId="179" formatCode="m/d/yy;@"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="180" formatCode="dd/mm/yyyy;@"/>
-    <numFmt numFmtId="181" formatCode="mmm\ d\,\ yyyy"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="m/d/yy;@"/>
+    <numFmt numFmtId="178" formatCode="ddd\,\ m/d/yyyy"/>
+    <numFmt numFmtId="179" formatCode="dd/mm/yyyy;@"/>
+    <numFmt numFmtId="180" formatCode="mmm\ d\,\ yyyy"/>
+    <numFmt numFmtId="181" formatCode="d"/>
   </numFmts>
   <fonts count="36">
     <font>
@@ -428,20 +425,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -455,9 +438,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -470,6 +459,22 @@
       <charset val="134"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
@@ -479,7 +484,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -510,24 +515,16 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -561,7 +558,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.15"/>
+        <fgColor theme="4" tint="0.8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -657,7 +654,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -669,25 +696,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -699,13 +708,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -723,55 +732,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -789,7 +762,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1165,6 +1162,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -1176,30 +1182,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1234,6 +1216,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -1247,11 +1244,11 @@
   </borders>
   <cellStyleXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="22" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="20" applyFont="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" applyFill="0">
@@ -1264,39 +1261,39 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="23" applyFill="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="28" borderId="32" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="23" applyFill="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="30" borderId="31" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="29" borderId="33" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="31" borderId="32" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" applyFill="0">
@@ -1306,99 +1303,99 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyProtection="0">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="20" borderId="29" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="25" borderId="30" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="30" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="22" borderId="33" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="24" borderId="29" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="22" borderId="30" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="31" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="29" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="35" fillId="0" borderId="34" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="20">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="20">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="134">
+  <cellXfs count="133">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1569,10 +1566,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="22" applyBorder="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="20" xfId="47" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="20" xfId="47">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="20" xfId="47" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="20" xfId="47">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
@@ -1597,10 +1594,10 @@
     <xf numFmtId="9" fontId="11" fillId="8" borderId="23" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="8" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="11" fillId="8" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="0" fillId="8" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="11" fillId="8" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1615,7 +1612,7 @@
     <xf numFmtId="9" fontId="11" fillId="9" borderId="23" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="0" fillId="9" borderId="23" xfId="11" applyNumberFormat="1" applyFill="1">
+    <xf numFmtId="179" fontId="0" fillId="9" borderId="23" xfId="11" applyNumberFormat="1" applyFill="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="11" fillId="9" borderId="23" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1630,10 +1627,10 @@
     <xf numFmtId="9" fontId="11" fillId="10" borderId="23" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="0" fillId="10" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="11" fillId="10" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="0" fillId="10" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="11" fillId="10" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="23" xfId="4" applyFill="1">
@@ -1645,10 +1642,7 @@
     <xf numFmtId="9" fontId="11" fillId="11" borderId="23" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="0" fillId="11" borderId="23" xfId="11" applyNumberFormat="1" applyFill="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="11" fillId="11" borderId="23" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="0" fillId="11" borderId="23" xfId="11" applyNumberFormat="1" applyFill="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="12" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1660,10 +1654,10 @@
     <xf numFmtId="9" fontId="11" fillId="12" borderId="23" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="12" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="11" fillId="12" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="0" fillId="12" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="11" fillId="12" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="23" xfId="4" applyFill="1">
@@ -1675,7 +1669,7 @@
     <xf numFmtId="9" fontId="11" fillId="13" borderId="23" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="13" borderId="23" xfId="11" applyFill="1">
+    <xf numFmtId="177" fontId="0" fillId="13" borderId="23" xfId="11" applyFill="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="14" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1687,10 +1681,10 @@
     <xf numFmtId="9" fontId="11" fillId="14" borderId="23" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="14" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="11" fillId="14" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="0" fillId="14" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="11" fillId="14" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="23" xfId="4" applyFill="1">
@@ -1702,7 +1696,7 @@
     <xf numFmtId="9" fontId="11" fillId="15" borderId="23" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="15" borderId="23" xfId="11" applyFill="1">
+    <xf numFmtId="177" fontId="0" fillId="15" borderId="23" xfId="11" applyFill="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="4">
@@ -1714,7 +1708,7 @@
     <xf numFmtId="9" fontId="11" fillId="0" borderId="23" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="23" xfId="11">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="23" xfId="11">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="16" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1726,10 +1720,10 @@
     <xf numFmtId="9" fontId="11" fillId="16" borderId="23" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="13" fillId="16" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="13" fillId="16" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="11" fillId="16" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="11" fillId="16" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="16" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1747,22 +1741,22 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="8" applyFont="1" applyProtection="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="181" fontId="0" fillId="17" borderId="24" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="0" fillId="17" borderId="24" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="181" fontId="0" fillId="17" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="0" fillId="17" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="181" fontId="0" fillId="17" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="0" fillId="17" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="178" fontId="18" fillId="17" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="18" fillId="17" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="18" fillId="17" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="181" fontId="18" fillId="17" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="181" fontId="18" fillId="17" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="181" fontId="18" fillId="17" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="18" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2348,12 +2342,12 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BL32"/>
+  <dimension ref="A1:BL31"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScalePageLayoutView="70" showRuler="0" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+    <sheetView showGridLines="0" zoomScalePageLayoutView="70" showRuler="0" workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="G16" sqref="G16"/>
+      <selection pane="bottomLeft" activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="30" customHeight="1"/>
@@ -2383,7 +2377,7 @@
       <c r="E1" s="56"/>
       <c r="F1" s="57"/>
       <c r="H1" s="55"/>
-      <c r="I1" s="122" t="s">
+      <c r="I1" s="121" t="s">
         <v>2</v>
       </c>
     </row>
@@ -2394,7 +2388,7 @@
       <c r="B2" s="58" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="123" t="s">
+      <c r="I2" s="122" t="s">
         <v>5</v>
       </c>
     </row>
@@ -2418,86 +2412,86 @@
         <v>45075</v>
       </c>
       <c r="F4" s="63"/>
-      <c r="I4" s="124">
+      <c r="I4" s="123">
         <f>I5</f>
         <v>45075</v>
       </c>
-      <c r="J4" s="125"/>
-      <c r="K4" s="125"/>
-      <c r="L4" s="125"/>
-      <c r="M4" s="125"/>
-      <c r="N4" s="125"/>
-      <c r="O4" s="126"/>
-      <c r="P4" s="124">
+      <c r="J4" s="124"/>
+      <c r="K4" s="124"/>
+      <c r="L4" s="124"/>
+      <c r="M4" s="124"/>
+      <c r="N4" s="124"/>
+      <c r="O4" s="125"/>
+      <c r="P4" s="123">
         <f>P5</f>
         <v>45082</v>
       </c>
-      <c r="Q4" s="125"/>
-      <c r="R4" s="125"/>
-      <c r="S4" s="125"/>
-      <c r="T4" s="125"/>
-      <c r="U4" s="125"/>
-      <c r="V4" s="126"/>
-      <c r="W4" s="124">
+      <c r="Q4" s="124"/>
+      <c r="R4" s="124"/>
+      <c r="S4" s="124"/>
+      <c r="T4" s="124"/>
+      <c r="U4" s="124"/>
+      <c r="V4" s="125"/>
+      <c r="W4" s="123">
         <f>W5</f>
         <v>45089</v>
       </c>
-      <c r="X4" s="125"/>
-      <c r="Y4" s="125"/>
-      <c r="Z4" s="125"/>
-      <c r="AA4" s="125"/>
-      <c r="AB4" s="125"/>
-      <c r="AC4" s="126"/>
-      <c r="AD4" s="124">
+      <c r="X4" s="124"/>
+      <c r="Y4" s="124"/>
+      <c r="Z4" s="124"/>
+      <c r="AA4" s="124"/>
+      <c r="AB4" s="124"/>
+      <c r="AC4" s="125"/>
+      <c r="AD4" s="123">
         <f>AD5</f>
         <v>45096</v>
       </c>
-      <c r="AE4" s="125"/>
-      <c r="AF4" s="125"/>
-      <c r="AG4" s="125"/>
-      <c r="AH4" s="125"/>
-      <c r="AI4" s="125"/>
-      <c r="AJ4" s="126"/>
-      <c r="AK4" s="124">
+      <c r="AE4" s="124"/>
+      <c r="AF4" s="124"/>
+      <c r="AG4" s="124"/>
+      <c r="AH4" s="124"/>
+      <c r="AI4" s="124"/>
+      <c r="AJ4" s="125"/>
+      <c r="AK4" s="123">
         <f>AK5</f>
         <v>45103</v>
       </c>
-      <c r="AL4" s="125"/>
-      <c r="AM4" s="125"/>
-      <c r="AN4" s="125"/>
-      <c r="AO4" s="125"/>
-      <c r="AP4" s="125"/>
-      <c r="AQ4" s="126"/>
-      <c r="AR4" s="124">
+      <c r="AL4" s="124"/>
+      <c r="AM4" s="124"/>
+      <c r="AN4" s="124"/>
+      <c r="AO4" s="124"/>
+      <c r="AP4" s="124"/>
+      <c r="AQ4" s="125"/>
+      <c r="AR4" s="123">
         <f>AR5</f>
         <v>45110</v>
       </c>
-      <c r="AS4" s="125"/>
-      <c r="AT4" s="125"/>
-      <c r="AU4" s="125"/>
-      <c r="AV4" s="125"/>
-      <c r="AW4" s="125"/>
-      <c r="AX4" s="126"/>
-      <c r="AY4" s="124">
+      <c r="AS4" s="124"/>
+      <c r="AT4" s="124"/>
+      <c r="AU4" s="124"/>
+      <c r="AV4" s="124"/>
+      <c r="AW4" s="124"/>
+      <c r="AX4" s="125"/>
+      <c r="AY4" s="123">
         <f>AY5</f>
         <v>45117</v>
       </c>
-      <c r="AZ4" s="125"/>
-      <c r="BA4" s="125"/>
-      <c r="BB4" s="125"/>
-      <c r="BC4" s="125"/>
-      <c r="BD4" s="125"/>
-      <c r="BE4" s="126"/>
-      <c r="BF4" s="124">
+      <c r="AZ4" s="124"/>
+      <c r="BA4" s="124"/>
+      <c r="BB4" s="124"/>
+      <c r="BC4" s="124"/>
+      <c r="BD4" s="124"/>
+      <c r="BE4" s="125"/>
+      <c r="BF4" s="123">
         <f>BF5</f>
         <v>45124</v>
       </c>
-      <c r="BG4" s="125"/>
-      <c r="BH4" s="125"/>
-      <c r="BI4" s="125"/>
-      <c r="BJ4" s="125"/>
-      <c r="BK4" s="125"/>
-      <c r="BL4" s="126"/>
+      <c r="BG4" s="124"/>
+      <c r="BH4" s="124"/>
+      <c r="BI4" s="124"/>
+      <c r="BJ4" s="124"/>
+      <c r="BK4" s="124"/>
+      <c r="BL4" s="125"/>
     </row>
     <row r="5" ht="15" customHeight="1" spans="1:64">
       <c r="A5" s="52" t="s">
@@ -2512,227 +2506,227 @@
         <v>1</v>
       </c>
       <c r="G5" s="64"/>
-      <c r="I5" s="127">
+      <c r="I5" s="126">
         <f>Project_Start-WEEKDAY(Project_Start,1)+2+7*(Display_Week-1)</f>
         <v>45075</v>
       </c>
-      <c r="J5" s="128">
+      <c r="J5" s="127">
         <f>I5+1</f>
         <v>45076</v>
       </c>
-      <c r="K5" s="128">
+      <c r="K5" s="127">
         <f t="shared" ref="K5:AZ5" si="0">J5+1</f>
         <v>45077</v>
       </c>
-      <c r="L5" s="128">
+      <c r="L5" s="127">
         <f t="shared" si="0"/>
         <v>45078</v>
       </c>
-      <c r="M5" s="128">
+      <c r="M5" s="127">
         <f t="shared" si="0"/>
         <v>45079</v>
       </c>
-      <c r="N5" s="128">
+      <c r="N5" s="127">
         <f t="shared" si="0"/>
         <v>45080</v>
       </c>
-      <c r="O5" s="129">
+      <c r="O5" s="128">
         <f t="shared" si="0"/>
         <v>45081</v>
       </c>
-      <c r="P5" s="127">
+      <c r="P5" s="126">
         <f t="shared" si="0"/>
         <v>45082</v>
       </c>
-      <c r="Q5" s="128">
+      <c r="Q5" s="127">
         <f t="shared" si="0"/>
         <v>45083</v>
       </c>
-      <c r="R5" s="128">
+      <c r="R5" s="127">
         <f t="shared" si="0"/>
         <v>45084</v>
       </c>
-      <c r="S5" s="128">
+      <c r="S5" s="127">
         <f t="shared" si="0"/>
         <v>45085</v>
       </c>
-      <c r="T5" s="128">
+      <c r="T5" s="127">
         <f t="shared" si="0"/>
         <v>45086</v>
       </c>
-      <c r="U5" s="128">
+      <c r="U5" s="127">
         <f t="shared" si="0"/>
         <v>45087</v>
       </c>
-      <c r="V5" s="129">
+      <c r="V5" s="128">
         <f t="shared" si="0"/>
         <v>45088</v>
       </c>
-      <c r="W5" s="127">
+      <c r="W5" s="126">
         <f t="shared" si="0"/>
         <v>45089</v>
       </c>
-      <c r="X5" s="128">
+      <c r="X5" s="127">
         <f t="shared" si="0"/>
         <v>45090</v>
       </c>
-      <c r="Y5" s="128">
+      <c r="Y5" s="127">
         <f t="shared" si="0"/>
         <v>45091</v>
       </c>
-      <c r="Z5" s="128">
+      <c r="Z5" s="127">
         <f t="shared" si="0"/>
         <v>45092</v>
       </c>
-      <c r="AA5" s="128">
+      <c r="AA5" s="127">
         <f t="shared" si="0"/>
         <v>45093</v>
       </c>
-      <c r="AB5" s="128">
+      <c r="AB5" s="127">
         <f t="shared" si="0"/>
         <v>45094</v>
       </c>
-      <c r="AC5" s="129">
+      <c r="AC5" s="128">
         <f t="shared" si="0"/>
         <v>45095</v>
       </c>
-      <c r="AD5" s="127">
+      <c r="AD5" s="126">
         <f t="shared" si="0"/>
         <v>45096</v>
       </c>
-      <c r="AE5" s="128">
+      <c r="AE5" s="127">
         <f t="shared" si="0"/>
         <v>45097</v>
       </c>
-      <c r="AF5" s="128">
+      <c r="AF5" s="127">
         <f t="shared" si="0"/>
         <v>45098</v>
       </c>
-      <c r="AG5" s="128">
+      <c r="AG5" s="127">
         <f t="shared" si="0"/>
         <v>45099</v>
       </c>
-      <c r="AH5" s="128">
+      <c r="AH5" s="127">
         <f t="shared" si="0"/>
         <v>45100</v>
       </c>
-      <c r="AI5" s="128">
+      <c r="AI5" s="127">
         <f t="shared" si="0"/>
         <v>45101</v>
       </c>
-      <c r="AJ5" s="129">
+      <c r="AJ5" s="128">
         <f t="shared" si="0"/>
         <v>45102</v>
       </c>
-      <c r="AK5" s="127">
+      <c r="AK5" s="126">
         <f t="shared" si="0"/>
         <v>45103</v>
       </c>
-      <c r="AL5" s="128">
+      <c r="AL5" s="127">
         <f t="shared" si="0"/>
         <v>45104</v>
       </c>
-      <c r="AM5" s="128">
+      <c r="AM5" s="127">
         <f t="shared" si="0"/>
         <v>45105</v>
       </c>
-      <c r="AN5" s="128">
+      <c r="AN5" s="127">
         <f t="shared" si="0"/>
         <v>45106</v>
       </c>
-      <c r="AO5" s="128">
+      <c r="AO5" s="127">
         <f t="shared" si="0"/>
         <v>45107</v>
       </c>
-      <c r="AP5" s="128">
+      <c r="AP5" s="127">
         <f t="shared" si="0"/>
         <v>45108</v>
       </c>
-      <c r="AQ5" s="129">
+      <c r="AQ5" s="128">
         <f t="shared" si="0"/>
         <v>45109</v>
       </c>
-      <c r="AR5" s="127">
+      <c r="AR5" s="126">
         <f t="shared" si="0"/>
         <v>45110</v>
       </c>
-      <c r="AS5" s="128">
+      <c r="AS5" s="127">
         <f t="shared" si="0"/>
         <v>45111</v>
       </c>
-      <c r="AT5" s="128">
+      <c r="AT5" s="127">
         <f t="shared" si="0"/>
         <v>45112</v>
       </c>
-      <c r="AU5" s="128">
+      <c r="AU5" s="127">
         <f t="shared" si="0"/>
         <v>45113</v>
       </c>
-      <c r="AV5" s="128">
+      <c r="AV5" s="127">
         <f t="shared" si="0"/>
         <v>45114</v>
       </c>
-      <c r="AW5" s="128">
+      <c r="AW5" s="127">
         <f t="shared" si="0"/>
         <v>45115</v>
       </c>
-      <c r="AX5" s="129">
+      <c r="AX5" s="128">
         <f t="shared" si="0"/>
         <v>45116</v>
       </c>
-      <c r="AY5" s="127">
+      <c r="AY5" s="126">
         <f t="shared" si="0"/>
         <v>45117</v>
       </c>
-      <c r="AZ5" s="128">
+      <c r="AZ5" s="127">
         <f t="shared" si="0"/>
         <v>45118</v>
       </c>
-      <c r="BA5" s="128">
+      <c r="BA5" s="127">
         <f t="shared" ref="BA5:BG5" si="1">AZ5+1</f>
         <v>45119</v>
       </c>
-      <c r="BB5" s="128">
+      <c r="BB5" s="127">
         <f t="shared" si="1"/>
         <v>45120</v>
       </c>
-      <c r="BC5" s="128">
+      <c r="BC5" s="127">
         <f t="shared" si="1"/>
         <v>45121</v>
       </c>
-      <c r="BD5" s="128">
+      <c r="BD5" s="127">
         <f t="shared" si="1"/>
         <v>45122</v>
       </c>
-      <c r="BE5" s="129">
+      <c r="BE5" s="128">
         <f t="shared" si="1"/>
         <v>45123</v>
       </c>
-      <c r="BF5" s="127">
+      <c r="BF5" s="126">
         <f t="shared" si="1"/>
         <v>45124</v>
       </c>
-      <c r="BG5" s="128">
+      <c r="BG5" s="127">
         <f t="shared" si="1"/>
         <v>45125</v>
       </c>
-      <c r="BH5" s="128">
+      <c r="BH5" s="127">
         <f t="shared" ref="BH5:BL5" si="2">BG5+1</f>
         <v>45126</v>
       </c>
-      <c r="BI5" s="128">
+      <c r="BI5" s="127">
         <f t="shared" si="2"/>
         <v>45127</v>
       </c>
-      <c r="BJ5" s="128">
+      <c r="BJ5" s="127">
         <f t="shared" si="2"/>
         <v>45128</v>
       </c>
-      <c r="BK5" s="128">
+      <c r="BK5" s="127">
         <f t="shared" si="2"/>
         <v>45129</v>
       </c>
-      <c r="BL5" s="129">
+      <c r="BL5" s="128">
         <f t="shared" si="2"/>
         <v>45130</v>
       </c>
@@ -2760,227 +2754,227 @@
       <c r="H6" s="67" t="s">
         <v>18</v>
       </c>
-      <c r="I6" s="130" t="str">
+      <c r="I6" s="129" t="str">
         <f t="shared" ref="I6" si="3">LEFT(TEXT(I5,"ddd"),1)</f>
         <v>M</v>
       </c>
-      <c r="J6" s="130" t="str">
+      <c r="J6" s="129" t="str">
         <f t="shared" ref="J6:AR6" si="4">LEFT(TEXT(J5,"ddd"),1)</f>
         <v>T</v>
       </c>
-      <c r="K6" s="130" t="str">
+      <c r="K6" s="129" t="str">
         <f t="shared" si="4"/>
         <v>W</v>
       </c>
-      <c r="L6" s="130" t="str">
+      <c r="L6" s="129" t="str">
         <f t="shared" si="4"/>
         <v>T</v>
       </c>
-      <c r="M6" s="130" t="str">
+      <c r="M6" s="129" t="str">
         <f t="shared" si="4"/>
         <v>F</v>
       </c>
-      <c r="N6" s="130" t="str">
+      <c r="N6" s="129" t="str">
         <f t="shared" si="4"/>
         <v>S</v>
       </c>
-      <c r="O6" s="130" t="str">
+      <c r="O6" s="129" t="str">
         <f t="shared" si="4"/>
         <v>S</v>
       </c>
-      <c r="P6" s="130" t="str">
+      <c r="P6" s="129" t="str">
         <f t="shared" si="4"/>
         <v>M</v>
       </c>
-      <c r="Q6" s="130" t="str">
+      <c r="Q6" s="129" t="str">
         <f t="shared" si="4"/>
         <v>T</v>
       </c>
-      <c r="R6" s="130" t="str">
+      <c r="R6" s="129" t="str">
         <f t="shared" si="4"/>
         <v>W</v>
       </c>
-      <c r="S6" s="130" t="str">
+      <c r="S6" s="129" t="str">
         <f t="shared" si="4"/>
         <v>T</v>
       </c>
-      <c r="T6" s="130" t="str">
+      <c r="T6" s="129" t="str">
         <f t="shared" si="4"/>
         <v>F</v>
       </c>
-      <c r="U6" s="130" t="str">
+      <c r="U6" s="129" t="str">
         <f t="shared" si="4"/>
         <v>S</v>
       </c>
-      <c r="V6" s="130" t="str">
+      <c r="V6" s="129" t="str">
         <f t="shared" si="4"/>
         <v>S</v>
       </c>
-      <c r="W6" s="130" t="str">
+      <c r="W6" s="129" t="str">
         <f t="shared" si="4"/>
         <v>M</v>
       </c>
-      <c r="X6" s="130" t="str">
+      <c r="X6" s="129" t="str">
         <f t="shared" si="4"/>
         <v>T</v>
       </c>
-      <c r="Y6" s="130" t="str">
+      <c r="Y6" s="129" t="str">
         <f t="shared" si="4"/>
         <v>W</v>
       </c>
-      <c r="Z6" s="130" t="str">
+      <c r="Z6" s="129" t="str">
         <f t="shared" si="4"/>
         <v>T</v>
       </c>
-      <c r="AA6" s="130" t="str">
+      <c r="AA6" s="129" t="str">
         <f t="shared" si="4"/>
         <v>F</v>
       </c>
-      <c r="AB6" s="130" t="str">
+      <c r="AB6" s="129" t="str">
         <f t="shared" si="4"/>
         <v>S</v>
       </c>
-      <c r="AC6" s="130" t="str">
+      <c r="AC6" s="129" t="str">
         <f t="shared" si="4"/>
         <v>S</v>
       </c>
-      <c r="AD6" s="130" t="str">
+      <c r="AD6" s="129" t="str">
         <f t="shared" si="4"/>
         <v>M</v>
       </c>
-      <c r="AE6" s="130" t="str">
+      <c r="AE6" s="129" t="str">
         <f t="shared" si="4"/>
         <v>T</v>
       </c>
-      <c r="AF6" s="130" t="str">
+      <c r="AF6" s="129" t="str">
         <f t="shared" si="4"/>
         <v>W</v>
       </c>
-      <c r="AG6" s="130" t="str">
+      <c r="AG6" s="129" t="str">
         <f t="shared" si="4"/>
         <v>T</v>
       </c>
-      <c r="AH6" s="130" t="str">
+      <c r="AH6" s="129" t="str">
         <f t="shared" si="4"/>
         <v>F</v>
       </c>
-      <c r="AI6" s="130" t="str">
+      <c r="AI6" s="129" t="str">
         <f t="shared" si="4"/>
         <v>S</v>
       </c>
-      <c r="AJ6" s="130" t="str">
+      <c r="AJ6" s="129" t="str">
         <f t="shared" si="4"/>
         <v>S</v>
       </c>
-      <c r="AK6" s="130" t="str">
+      <c r="AK6" s="129" t="str">
         <f t="shared" si="4"/>
         <v>M</v>
       </c>
-      <c r="AL6" s="130" t="str">
+      <c r="AL6" s="129" t="str">
         <f t="shared" si="4"/>
         <v>T</v>
       </c>
-      <c r="AM6" s="130" t="str">
+      <c r="AM6" s="129" t="str">
         <f t="shared" si="4"/>
         <v>W</v>
       </c>
-      <c r="AN6" s="130" t="str">
+      <c r="AN6" s="129" t="str">
         <f t="shared" si="4"/>
         <v>T</v>
       </c>
-      <c r="AO6" s="130" t="str">
+      <c r="AO6" s="129" t="str">
         <f t="shared" si="4"/>
         <v>F</v>
       </c>
-      <c r="AP6" s="130" t="str">
+      <c r="AP6" s="129" t="str">
         <f t="shared" si="4"/>
         <v>S</v>
       </c>
-      <c r="AQ6" s="130" t="str">
+      <c r="AQ6" s="129" t="str">
         <f t="shared" si="4"/>
         <v>S</v>
       </c>
-      <c r="AR6" s="130" t="str">
+      <c r="AR6" s="129" t="str">
         <f t="shared" si="4"/>
         <v>M</v>
       </c>
-      <c r="AS6" s="130" t="str">
+      <c r="AS6" s="129" t="str">
         <f t="shared" ref="AS6:BL6" si="5">LEFT(TEXT(AS5,"ddd"),1)</f>
         <v>T</v>
       </c>
-      <c r="AT6" s="130" t="str">
+      <c r="AT6" s="129" t="str">
         <f t="shared" si="5"/>
         <v>W</v>
       </c>
-      <c r="AU6" s="130" t="str">
+      <c r="AU6" s="129" t="str">
         <f t="shared" si="5"/>
         <v>T</v>
       </c>
-      <c r="AV6" s="130" t="str">
+      <c r="AV6" s="129" t="str">
         <f t="shared" si="5"/>
         <v>F</v>
       </c>
-      <c r="AW6" s="130" t="str">
+      <c r="AW6" s="129" t="str">
         <f t="shared" si="5"/>
         <v>S</v>
       </c>
-      <c r="AX6" s="130" t="str">
+      <c r="AX6" s="129" t="str">
         <f t="shared" si="5"/>
         <v>S</v>
       </c>
-      <c r="AY6" s="130" t="str">
+      <c r="AY6" s="129" t="str">
         <f t="shared" si="5"/>
         <v>M</v>
       </c>
-      <c r="AZ6" s="130" t="str">
+      <c r="AZ6" s="129" t="str">
         <f t="shared" si="5"/>
         <v>T</v>
       </c>
-      <c r="BA6" s="130" t="str">
+      <c r="BA6" s="129" t="str">
         <f t="shared" si="5"/>
         <v>W</v>
       </c>
-      <c r="BB6" s="130" t="str">
+      <c r="BB6" s="129" t="str">
         <f t="shared" si="5"/>
         <v>T</v>
       </c>
-      <c r="BC6" s="130" t="str">
+      <c r="BC6" s="129" t="str">
         <f t="shared" si="5"/>
         <v>F</v>
       </c>
-      <c r="BD6" s="130" t="str">
+      <c r="BD6" s="129" t="str">
         <f t="shared" si="5"/>
         <v>S</v>
       </c>
-      <c r="BE6" s="130" t="str">
+      <c r="BE6" s="129" t="str">
         <f t="shared" si="5"/>
         <v>S</v>
       </c>
-      <c r="BF6" s="130" t="str">
+      <c r="BF6" s="129" t="str">
         <f t="shared" si="5"/>
         <v>M</v>
       </c>
-      <c r="BG6" s="130" t="str">
+      <c r="BG6" s="129" t="str">
         <f t="shared" si="5"/>
         <v>T</v>
       </c>
-      <c r="BH6" s="130" t="str">
+      <c r="BH6" s="129" t="str">
         <f t="shared" si="5"/>
         <v>W</v>
       </c>
-      <c r="BI6" s="130" t="str">
+      <c r="BI6" s="129" t="str">
         <f t="shared" si="5"/>
         <v>T</v>
       </c>
-      <c r="BJ6" s="130" t="str">
+      <c r="BJ6" s="129" t="str">
         <f t="shared" si="5"/>
         <v>F</v>
       </c>
-      <c r="BK6" s="130" t="str">
+      <c r="BK6" s="129" t="str">
         <f t="shared" si="5"/>
         <v>S</v>
       </c>
-      <c r="BL6" s="130" t="str">
+      <c r="BL6" s="129" t="str">
         <f t="shared" si="5"/>
         <v>S</v>
       </c>
@@ -2995,62 +2989,62 @@
         <f>IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
         <v/>
       </c>
-      <c r="I7" s="131"/>
-      <c r="J7" s="131"/>
-      <c r="K7" s="131"/>
-      <c r="L7" s="131"/>
-      <c r="M7" s="131"/>
-      <c r="N7" s="131"/>
-      <c r="O7" s="131"/>
-      <c r="P7" s="131"/>
-      <c r="Q7" s="131"/>
-      <c r="R7" s="131"/>
-      <c r="S7" s="131"/>
-      <c r="T7" s="131"/>
-      <c r="U7" s="131"/>
-      <c r="V7" s="131"/>
-      <c r="W7" s="131"/>
-      <c r="X7" s="131"/>
-      <c r="Y7" s="131"/>
-      <c r="Z7" s="131"/>
-      <c r="AA7" s="131"/>
-      <c r="AB7" s="131"/>
-      <c r="AC7" s="131"/>
-      <c r="AD7" s="131"/>
-      <c r="AE7" s="131"/>
-      <c r="AF7" s="131"/>
-      <c r="AG7" s="131"/>
-      <c r="AH7" s="131"/>
-      <c r="AI7" s="131"/>
-      <c r="AJ7" s="131"/>
-      <c r="AK7" s="131"/>
-      <c r="AL7" s="131"/>
-      <c r="AM7" s="131"/>
-      <c r="AN7" s="131"/>
-      <c r="AO7" s="131"/>
-      <c r="AP7" s="131"/>
-      <c r="AQ7" s="131"/>
-      <c r="AR7" s="131"/>
-      <c r="AS7" s="131"/>
-      <c r="AT7" s="131"/>
-      <c r="AU7" s="131"/>
-      <c r="AV7" s="131"/>
-      <c r="AW7" s="131"/>
-      <c r="AX7" s="131"/>
-      <c r="AY7" s="131"/>
-      <c r="AZ7" s="131"/>
-      <c r="BA7" s="131"/>
-      <c r="BB7" s="131"/>
-      <c r="BC7" s="131"/>
-      <c r="BD7" s="131"/>
-      <c r="BE7" s="131"/>
-      <c r="BF7" s="131"/>
-      <c r="BG7" s="131"/>
-      <c r="BH7" s="131"/>
-      <c r="BI7" s="131"/>
-      <c r="BJ7" s="131"/>
-      <c r="BK7" s="131"/>
-      <c r="BL7" s="131"/>
+      <c r="I7" s="130"/>
+      <c r="J7" s="130"/>
+      <c r="K7" s="130"/>
+      <c r="L7" s="130"/>
+      <c r="M7" s="130"/>
+      <c r="N7" s="130"/>
+      <c r="O7" s="130"/>
+      <c r="P7" s="130"/>
+      <c r="Q7" s="130"/>
+      <c r="R7" s="130"/>
+      <c r="S7" s="130"/>
+      <c r="T7" s="130"/>
+      <c r="U7" s="130"/>
+      <c r="V7" s="130"/>
+      <c r="W7" s="130"/>
+      <c r="X7" s="130"/>
+      <c r="Y7" s="130"/>
+      <c r="Z7" s="130"/>
+      <c r="AA7" s="130"/>
+      <c r="AB7" s="130"/>
+      <c r="AC7" s="130"/>
+      <c r="AD7" s="130"/>
+      <c r="AE7" s="130"/>
+      <c r="AF7" s="130"/>
+      <c r="AG7" s="130"/>
+      <c r="AH7" s="130"/>
+      <c r="AI7" s="130"/>
+      <c r="AJ7" s="130"/>
+      <c r="AK7" s="130"/>
+      <c r="AL7" s="130"/>
+      <c r="AM7" s="130"/>
+      <c r="AN7" s="130"/>
+      <c r="AO7" s="130"/>
+      <c r="AP7" s="130"/>
+      <c r="AQ7" s="130"/>
+      <c r="AR7" s="130"/>
+      <c r="AS7" s="130"/>
+      <c r="AT7" s="130"/>
+      <c r="AU7" s="130"/>
+      <c r="AV7" s="130"/>
+      <c r="AW7" s="130"/>
+      <c r="AX7" s="130"/>
+      <c r="AY7" s="130"/>
+      <c r="AZ7" s="130"/>
+      <c r="BA7" s="130"/>
+      <c r="BB7" s="130"/>
+      <c r="BC7" s="130"/>
+      <c r="BD7" s="130"/>
+      <c r="BE7" s="130"/>
+      <c r="BF7" s="130"/>
+      <c r="BG7" s="130"/>
+      <c r="BH7" s="130"/>
+      <c r="BI7" s="130"/>
+      <c r="BJ7" s="130"/>
+      <c r="BK7" s="130"/>
+      <c r="BL7" s="130"/>
     </row>
     <row r="8" s="50" customFormat="1" customHeight="1" spans="1:64">
       <c r="A8" s="52" t="s">
@@ -3068,62 +3062,62 @@
         <f>IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
         <v/>
       </c>
-      <c r="I8" s="131"/>
-      <c r="J8" s="131"/>
-      <c r="K8" s="131"/>
-      <c r="L8" s="131"/>
-      <c r="M8" s="131"/>
-      <c r="N8" s="131"/>
-      <c r="O8" s="131"/>
-      <c r="P8" s="131"/>
-      <c r="Q8" s="131"/>
-      <c r="R8" s="131"/>
-      <c r="S8" s="131"/>
-      <c r="T8" s="131"/>
-      <c r="U8" s="131"/>
-      <c r="V8" s="131"/>
-      <c r="W8" s="131"/>
-      <c r="X8" s="131"/>
-      <c r="Y8" s="131"/>
-      <c r="Z8" s="131"/>
-      <c r="AA8" s="131"/>
-      <c r="AB8" s="131"/>
-      <c r="AC8" s="131"/>
-      <c r="AD8" s="131"/>
-      <c r="AE8" s="131"/>
-      <c r="AF8" s="131"/>
-      <c r="AG8" s="131"/>
-      <c r="AH8" s="131"/>
-      <c r="AI8" s="131"/>
-      <c r="AJ8" s="131"/>
-      <c r="AK8" s="131"/>
-      <c r="AL8" s="131"/>
-      <c r="AM8" s="131"/>
-      <c r="AN8" s="131"/>
-      <c r="AO8" s="131"/>
-      <c r="AP8" s="131"/>
-      <c r="AQ8" s="131"/>
-      <c r="AR8" s="131"/>
-      <c r="AS8" s="131"/>
-      <c r="AT8" s="131"/>
-      <c r="AU8" s="131"/>
-      <c r="AV8" s="131"/>
-      <c r="AW8" s="131"/>
-      <c r="AX8" s="131"/>
-      <c r="AY8" s="131"/>
-      <c r="AZ8" s="131"/>
-      <c r="BA8" s="131"/>
-      <c r="BB8" s="131"/>
-      <c r="BC8" s="131"/>
-      <c r="BD8" s="131"/>
-      <c r="BE8" s="131"/>
-      <c r="BF8" s="131"/>
-      <c r="BG8" s="131"/>
-      <c r="BH8" s="131"/>
-      <c r="BI8" s="131"/>
-      <c r="BJ8" s="131"/>
-      <c r="BK8" s="131"/>
-      <c r="BL8" s="131"/>
+      <c r="I8" s="130"/>
+      <c r="J8" s="130"/>
+      <c r="K8" s="130"/>
+      <c r="L8" s="130"/>
+      <c r="M8" s="130"/>
+      <c r="N8" s="130"/>
+      <c r="O8" s="130"/>
+      <c r="P8" s="130"/>
+      <c r="Q8" s="130"/>
+      <c r="R8" s="130"/>
+      <c r="S8" s="130"/>
+      <c r="T8" s="130"/>
+      <c r="U8" s="130"/>
+      <c r="V8" s="130"/>
+      <c r="W8" s="130"/>
+      <c r="X8" s="130"/>
+      <c r="Y8" s="130"/>
+      <c r="Z8" s="130"/>
+      <c r="AA8" s="130"/>
+      <c r="AB8" s="130"/>
+      <c r="AC8" s="130"/>
+      <c r="AD8" s="130"/>
+      <c r="AE8" s="130"/>
+      <c r="AF8" s="130"/>
+      <c r="AG8" s="130"/>
+      <c r="AH8" s="130"/>
+      <c r="AI8" s="130"/>
+      <c r="AJ8" s="130"/>
+      <c r="AK8" s="130"/>
+      <c r="AL8" s="130"/>
+      <c r="AM8" s="130"/>
+      <c r="AN8" s="130"/>
+      <c r="AO8" s="130"/>
+      <c r="AP8" s="130"/>
+      <c r="AQ8" s="130"/>
+      <c r="AR8" s="130"/>
+      <c r="AS8" s="130"/>
+      <c r="AT8" s="130"/>
+      <c r="AU8" s="130"/>
+      <c r="AV8" s="130"/>
+      <c r="AW8" s="130"/>
+      <c r="AX8" s="130"/>
+      <c r="AY8" s="130"/>
+      <c r="AZ8" s="130"/>
+      <c r="BA8" s="130"/>
+      <c r="BB8" s="130"/>
+      <c r="BC8" s="130"/>
+      <c r="BD8" s="130"/>
+      <c r="BE8" s="130"/>
+      <c r="BF8" s="130"/>
+      <c r="BG8" s="130"/>
+      <c r="BH8" s="130"/>
+      <c r="BI8" s="130"/>
+      <c r="BJ8" s="130"/>
+      <c r="BK8" s="130"/>
+      <c r="BL8" s="130"/>
     </row>
     <row r="9" s="50" customFormat="1" customHeight="1" spans="1:64">
       <c r="A9" s="52" t="s">
@@ -3151,62 +3145,62 @@
         <f>IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
         <v>1</v>
       </c>
-      <c r="I9" s="131"/>
-      <c r="J9" s="131"/>
-      <c r="K9" s="131"/>
-      <c r="L9" s="131"/>
-      <c r="M9" s="131"/>
-      <c r="N9" s="131"/>
-      <c r="O9" s="131"/>
-      <c r="P9" s="131"/>
-      <c r="Q9" s="131"/>
-      <c r="R9" s="131"/>
-      <c r="S9" s="131"/>
-      <c r="T9" s="131"/>
-      <c r="U9" s="131"/>
-      <c r="V9" s="131"/>
-      <c r="W9" s="131"/>
-      <c r="X9" s="131"/>
-      <c r="Y9" s="131"/>
-      <c r="Z9" s="131"/>
-      <c r="AA9" s="131"/>
-      <c r="AB9" s="131"/>
-      <c r="AC9" s="131"/>
-      <c r="AD9" s="131"/>
-      <c r="AE9" s="131"/>
-      <c r="AF9" s="131"/>
-      <c r="AG9" s="131"/>
-      <c r="AH9" s="131"/>
-      <c r="AI9" s="131"/>
-      <c r="AJ9" s="131"/>
-      <c r="AK9" s="131"/>
-      <c r="AL9" s="131"/>
-      <c r="AM9" s="131"/>
-      <c r="AN9" s="131"/>
-      <c r="AO9" s="131"/>
-      <c r="AP9" s="131"/>
-      <c r="AQ9" s="131"/>
-      <c r="AR9" s="131"/>
-      <c r="AS9" s="131"/>
-      <c r="AT9" s="131"/>
-      <c r="AU9" s="131"/>
-      <c r="AV9" s="131"/>
-      <c r="AW9" s="131"/>
-      <c r="AX9" s="131"/>
-      <c r="AY9" s="131"/>
-      <c r="AZ9" s="131"/>
-      <c r="BA9" s="131"/>
-      <c r="BB9" s="131"/>
-      <c r="BC9" s="131"/>
-      <c r="BD9" s="131"/>
-      <c r="BE9" s="131"/>
-      <c r="BF9" s="131"/>
-      <c r="BG9" s="131"/>
-      <c r="BH9" s="131"/>
-      <c r="BI9" s="131"/>
-      <c r="BJ9" s="131"/>
-      <c r="BK9" s="131"/>
-      <c r="BL9" s="131"/>
+      <c r="I9" s="130"/>
+      <c r="J9" s="130"/>
+      <c r="K9" s="130"/>
+      <c r="L9" s="130"/>
+      <c r="M9" s="130"/>
+      <c r="N9" s="130"/>
+      <c r="O9" s="130"/>
+      <c r="P9" s="130"/>
+      <c r="Q9" s="130"/>
+      <c r="R9" s="130"/>
+      <c r="S9" s="130"/>
+      <c r="T9" s="130"/>
+      <c r="U9" s="130"/>
+      <c r="V9" s="130"/>
+      <c r="W9" s="130"/>
+      <c r="X9" s="130"/>
+      <c r="Y9" s="130"/>
+      <c r="Z9" s="130"/>
+      <c r="AA9" s="130"/>
+      <c r="AB9" s="130"/>
+      <c r="AC9" s="130"/>
+      <c r="AD9" s="130"/>
+      <c r="AE9" s="130"/>
+      <c r="AF9" s="130"/>
+      <c r="AG9" s="130"/>
+      <c r="AH9" s="130"/>
+      <c r="AI9" s="130"/>
+      <c r="AJ9" s="130"/>
+      <c r="AK9" s="130"/>
+      <c r="AL9" s="130"/>
+      <c r="AM9" s="130"/>
+      <c r="AN9" s="130"/>
+      <c r="AO9" s="130"/>
+      <c r="AP9" s="130"/>
+      <c r="AQ9" s="130"/>
+      <c r="AR9" s="130"/>
+      <c r="AS9" s="130"/>
+      <c r="AT9" s="130"/>
+      <c r="AU9" s="130"/>
+      <c r="AV9" s="130"/>
+      <c r="AW9" s="130"/>
+      <c r="AX9" s="130"/>
+      <c r="AY9" s="130"/>
+      <c r="AZ9" s="130"/>
+      <c r="BA9" s="130"/>
+      <c r="BB9" s="130"/>
+      <c r="BC9" s="130"/>
+      <c r="BD9" s="130"/>
+      <c r="BE9" s="130"/>
+      <c r="BF9" s="130"/>
+      <c r="BG9" s="130"/>
+      <c r="BH9" s="130"/>
+      <c r="BI9" s="130"/>
+      <c r="BJ9" s="130"/>
+      <c r="BK9" s="130"/>
+      <c r="BL9" s="130"/>
     </row>
     <row r="10" s="50" customFormat="1" customHeight="1" spans="1:64">
       <c r="A10" s="52" t="s">
@@ -3232,62 +3226,62 @@
         <f>IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
         <v>1</v>
       </c>
-      <c r="I10" s="131"/>
-      <c r="J10" s="131"/>
-      <c r="K10" s="131"/>
-      <c r="L10" s="131"/>
-      <c r="M10" s="131"/>
-      <c r="N10" s="131"/>
-      <c r="O10" s="131"/>
-      <c r="P10" s="131"/>
-      <c r="Q10" s="131"/>
-      <c r="R10" s="131"/>
-      <c r="S10" s="131"/>
-      <c r="T10" s="131"/>
-      <c r="U10" s="133"/>
-      <c r="V10" s="133"/>
-      <c r="W10" s="131"/>
-      <c r="X10" s="131"/>
-      <c r="Y10" s="131"/>
-      <c r="Z10" s="131"/>
-      <c r="AA10" s="131"/>
-      <c r="AB10" s="131"/>
-      <c r="AC10" s="131"/>
-      <c r="AD10" s="131"/>
-      <c r="AE10" s="131"/>
-      <c r="AF10" s="131"/>
-      <c r="AG10" s="131"/>
-      <c r="AH10" s="131"/>
-      <c r="AI10" s="131"/>
-      <c r="AJ10" s="131"/>
-      <c r="AK10" s="131"/>
-      <c r="AL10" s="131"/>
-      <c r="AM10" s="131"/>
-      <c r="AN10" s="131"/>
-      <c r="AO10" s="131"/>
-      <c r="AP10" s="131"/>
-      <c r="AQ10" s="131"/>
-      <c r="AR10" s="131"/>
-      <c r="AS10" s="131"/>
-      <c r="AT10" s="131"/>
-      <c r="AU10" s="131"/>
-      <c r="AV10" s="131"/>
-      <c r="AW10" s="131"/>
-      <c r="AX10" s="131"/>
-      <c r="AY10" s="131"/>
-      <c r="AZ10" s="131"/>
-      <c r="BA10" s="131"/>
-      <c r="BB10" s="131"/>
-      <c r="BC10" s="131"/>
-      <c r="BD10" s="131"/>
-      <c r="BE10" s="131"/>
-      <c r="BF10" s="131"/>
-      <c r="BG10" s="131"/>
-      <c r="BH10" s="131"/>
-      <c r="BI10" s="131"/>
-      <c r="BJ10" s="131"/>
-      <c r="BK10" s="131"/>
-      <c r="BL10" s="131"/>
+      <c r="I10" s="130"/>
+      <c r="J10" s="130"/>
+      <c r="K10" s="130"/>
+      <c r="L10" s="130"/>
+      <c r="M10" s="130"/>
+      <c r="N10" s="130"/>
+      <c r="O10" s="130"/>
+      <c r="P10" s="130"/>
+      <c r="Q10" s="130"/>
+      <c r="R10" s="130"/>
+      <c r="S10" s="130"/>
+      <c r="T10" s="130"/>
+      <c r="U10" s="132"/>
+      <c r="V10" s="132"/>
+      <c r="W10" s="130"/>
+      <c r="X10" s="130"/>
+      <c r="Y10" s="130"/>
+      <c r="Z10" s="130"/>
+      <c r="AA10" s="130"/>
+      <c r="AB10" s="130"/>
+      <c r="AC10" s="130"/>
+      <c r="AD10" s="130"/>
+      <c r="AE10" s="130"/>
+      <c r="AF10" s="130"/>
+      <c r="AG10" s="130"/>
+      <c r="AH10" s="130"/>
+      <c r="AI10" s="130"/>
+      <c r="AJ10" s="130"/>
+      <c r="AK10" s="130"/>
+      <c r="AL10" s="130"/>
+      <c r="AM10" s="130"/>
+      <c r="AN10" s="130"/>
+      <c r="AO10" s="130"/>
+      <c r="AP10" s="130"/>
+      <c r="AQ10" s="130"/>
+      <c r="AR10" s="130"/>
+      <c r="AS10" s="130"/>
+      <c r="AT10" s="130"/>
+      <c r="AU10" s="130"/>
+      <c r="AV10" s="130"/>
+      <c r="AW10" s="130"/>
+      <c r="AX10" s="130"/>
+      <c r="AY10" s="130"/>
+      <c r="AZ10" s="130"/>
+      <c r="BA10" s="130"/>
+      <c r="BB10" s="130"/>
+      <c r="BC10" s="130"/>
+      <c r="BD10" s="130"/>
+      <c r="BE10" s="130"/>
+      <c r="BF10" s="130"/>
+      <c r="BG10" s="130"/>
+      <c r="BH10" s="130"/>
+      <c r="BI10" s="130"/>
+      <c r="BJ10" s="130"/>
+      <c r="BK10" s="130"/>
+      <c r="BL10" s="130"/>
     </row>
     <row r="11" s="50" customFormat="1" customHeight="1" spans="1:64">
       <c r="A11" s="52" t="s">
@@ -3305,62 +3299,62 @@
         <f>IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
         <v/>
       </c>
-      <c r="I11" s="131"/>
-      <c r="J11" s="131"/>
-      <c r="K11" s="131"/>
-      <c r="L11" s="131"/>
-      <c r="M11" s="131"/>
-      <c r="N11" s="131"/>
-      <c r="O11" s="131"/>
-      <c r="P11" s="131"/>
-      <c r="Q11" s="131"/>
-      <c r="R11" s="131"/>
-      <c r="S11" s="131"/>
-      <c r="T11" s="131"/>
-      <c r="U11" s="131"/>
-      <c r="V11" s="131"/>
-      <c r="W11" s="131"/>
-      <c r="X11" s="131"/>
-      <c r="Y11" s="131"/>
-      <c r="Z11" s="131"/>
-      <c r="AA11" s="131"/>
-      <c r="AB11" s="131"/>
-      <c r="AC11" s="131"/>
-      <c r="AD11" s="131"/>
-      <c r="AE11" s="131"/>
-      <c r="AF11" s="131"/>
-      <c r="AG11" s="131"/>
-      <c r="AH11" s="131"/>
-      <c r="AI11" s="131"/>
-      <c r="AJ11" s="131"/>
-      <c r="AK11" s="131"/>
-      <c r="AL11" s="131"/>
-      <c r="AM11" s="131"/>
-      <c r="AN11" s="131"/>
-      <c r="AO11" s="131"/>
-      <c r="AP11" s="131"/>
-      <c r="AQ11" s="131"/>
-      <c r="AR11" s="131"/>
-      <c r="AS11" s="131"/>
-      <c r="AT11" s="131"/>
-      <c r="AU11" s="131"/>
-      <c r="AV11" s="131"/>
-      <c r="AW11" s="131"/>
-      <c r="AX11" s="131"/>
-      <c r="AY11" s="131"/>
-      <c r="AZ11" s="131"/>
-      <c r="BA11" s="131"/>
-      <c r="BB11" s="131"/>
-      <c r="BC11" s="131"/>
-      <c r="BD11" s="131"/>
-      <c r="BE11" s="131"/>
-      <c r="BF11" s="131"/>
-      <c r="BG11" s="131"/>
-      <c r="BH11" s="131"/>
-      <c r="BI11" s="131"/>
-      <c r="BJ11" s="131"/>
-      <c r="BK11" s="131"/>
-      <c r="BL11" s="131"/>
+      <c r="I11" s="130"/>
+      <c r="J11" s="130"/>
+      <c r="K11" s="130"/>
+      <c r="L11" s="130"/>
+      <c r="M11" s="130"/>
+      <c r="N11" s="130"/>
+      <c r="O11" s="130"/>
+      <c r="P11" s="130"/>
+      <c r="Q11" s="130"/>
+      <c r="R11" s="130"/>
+      <c r="S11" s="130"/>
+      <c r="T11" s="130"/>
+      <c r="U11" s="130"/>
+      <c r="V11" s="130"/>
+      <c r="W11" s="130"/>
+      <c r="X11" s="130"/>
+      <c r="Y11" s="130"/>
+      <c r="Z11" s="130"/>
+      <c r="AA11" s="130"/>
+      <c r="AB11" s="130"/>
+      <c r="AC11" s="130"/>
+      <c r="AD11" s="130"/>
+      <c r="AE11" s="130"/>
+      <c r="AF11" s="130"/>
+      <c r="AG11" s="130"/>
+      <c r="AH11" s="130"/>
+      <c r="AI11" s="130"/>
+      <c r="AJ11" s="130"/>
+      <c r="AK11" s="130"/>
+      <c r="AL11" s="130"/>
+      <c r="AM11" s="130"/>
+      <c r="AN11" s="130"/>
+      <c r="AO11" s="130"/>
+      <c r="AP11" s="130"/>
+      <c r="AQ11" s="130"/>
+      <c r="AR11" s="130"/>
+      <c r="AS11" s="130"/>
+      <c r="AT11" s="130"/>
+      <c r="AU11" s="130"/>
+      <c r="AV11" s="130"/>
+      <c r="AW11" s="130"/>
+      <c r="AX11" s="130"/>
+      <c r="AY11" s="130"/>
+      <c r="AZ11" s="130"/>
+      <c r="BA11" s="130"/>
+      <c r="BB11" s="130"/>
+      <c r="BC11" s="130"/>
+      <c r="BD11" s="130"/>
+      <c r="BE11" s="130"/>
+      <c r="BF11" s="130"/>
+      <c r="BG11" s="130"/>
+      <c r="BH11" s="130"/>
+      <c r="BI11" s="130"/>
+      <c r="BJ11" s="130"/>
+      <c r="BK11" s="130"/>
+      <c r="BL11" s="130"/>
     </row>
     <row r="12" s="50" customFormat="1" customHeight="1" spans="1:64">
       <c r="A12" s="52"/>
@@ -3384,62 +3378,62 @@
         <f>IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
         <v>2</v>
       </c>
-      <c r="I12" s="131"/>
-      <c r="J12" s="131"/>
-      <c r="K12" s="131"/>
-      <c r="L12" s="131"/>
-      <c r="M12" s="131"/>
-      <c r="N12" s="131"/>
-      <c r="O12" s="131"/>
-      <c r="P12" s="131"/>
-      <c r="Q12" s="131"/>
-      <c r="R12" s="131"/>
-      <c r="S12" s="131"/>
-      <c r="T12" s="131"/>
-      <c r="U12" s="131"/>
-      <c r="V12" s="131"/>
-      <c r="W12" s="131"/>
-      <c r="X12" s="131"/>
-      <c r="Y12" s="131"/>
-      <c r="Z12" s="131"/>
-      <c r="AA12" s="131"/>
-      <c r="AB12" s="131"/>
-      <c r="AC12" s="131"/>
-      <c r="AD12" s="131"/>
-      <c r="AE12" s="131"/>
-      <c r="AF12" s="131"/>
-      <c r="AG12" s="131"/>
-      <c r="AH12" s="131"/>
-      <c r="AI12" s="131"/>
-      <c r="AJ12" s="131"/>
-      <c r="AK12" s="131"/>
-      <c r="AL12" s="131"/>
-      <c r="AM12" s="131"/>
-      <c r="AN12" s="131"/>
-      <c r="AO12" s="131"/>
-      <c r="AP12" s="131"/>
-      <c r="AQ12" s="131"/>
-      <c r="AR12" s="131"/>
-      <c r="AS12" s="131"/>
-      <c r="AT12" s="131"/>
-      <c r="AU12" s="131"/>
-      <c r="AV12" s="131"/>
-      <c r="AW12" s="131"/>
-      <c r="AX12" s="131"/>
-      <c r="AY12" s="131"/>
-      <c r="AZ12" s="131"/>
-      <c r="BA12" s="131"/>
-      <c r="BB12" s="131"/>
-      <c r="BC12" s="131"/>
-      <c r="BD12" s="131"/>
-      <c r="BE12" s="131"/>
-      <c r="BF12" s="131"/>
-      <c r="BG12" s="131"/>
-      <c r="BH12" s="131"/>
-      <c r="BI12" s="131"/>
-      <c r="BJ12" s="131"/>
-      <c r="BK12" s="131"/>
-      <c r="BL12" s="131"/>
+      <c r="I12" s="130"/>
+      <c r="J12" s="130"/>
+      <c r="K12" s="130"/>
+      <c r="L12" s="130"/>
+      <c r="M12" s="130"/>
+      <c r="N12" s="130"/>
+      <c r="O12" s="130"/>
+      <c r="P12" s="130"/>
+      <c r="Q12" s="130"/>
+      <c r="R12" s="130"/>
+      <c r="S12" s="130"/>
+      <c r="T12" s="130"/>
+      <c r="U12" s="130"/>
+      <c r="V12" s="130"/>
+      <c r="W12" s="130"/>
+      <c r="X12" s="130"/>
+      <c r="Y12" s="130"/>
+      <c r="Z12" s="130"/>
+      <c r="AA12" s="130"/>
+      <c r="AB12" s="130"/>
+      <c r="AC12" s="130"/>
+      <c r="AD12" s="130"/>
+      <c r="AE12" s="130"/>
+      <c r="AF12" s="130"/>
+      <c r="AG12" s="130"/>
+      <c r="AH12" s="130"/>
+      <c r="AI12" s="130"/>
+      <c r="AJ12" s="130"/>
+      <c r="AK12" s="130"/>
+      <c r="AL12" s="130"/>
+      <c r="AM12" s="130"/>
+      <c r="AN12" s="130"/>
+      <c r="AO12" s="130"/>
+      <c r="AP12" s="130"/>
+      <c r="AQ12" s="130"/>
+      <c r="AR12" s="130"/>
+      <c r="AS12" s="130"/>
+      <c r="AT12" s="130"/>
+      <c r="AU12" s="130"/>
+      <c r="AV12" s="130"/>
+      <c r="AW12" s="130"/>
+      <c r="AX12" s="130"/>
+      <c r="AY12" s="130"/>
+      <c r="AZ12" s="130"/>
+      <c r="BA12" s="130"/>
+      <c r="BB12" s="130"/>
+      <c r="BC12" s="130"/>
+      <c r="BD12" s="130"/>
+      <c r="BE12" s="130"/>
+      <c r="BF12" s="130"/>
+      <c r="BG12" s="130"/>
+      <c r="BH12" s="130"/>
+      <c r="BI12" s="130"/>
+      <c r="BJ12" s="130"/>
+      <c r="BK12" s="130"/>
+      <c r="BL12" s="130"/>
     </row>
     <row r="13" s="50" customFormat="1" customHeight="1" spans="1:64">
       <c r="A13" s="51"/>
@@ -3447,7 +3441,7 @@
         <v>30</v>
       </c>
       <c r="C13" s="86"/>
-      <c r="D13" s="89">
+      <c r="D13" s="87">
         <v>0</v>
       </c>
       <c r="E13" s="88">
@@ -3463,62 +3457,62 @@
         <f>IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
         <v>2</v>
       </c>
-      <c r="I13" s="131"/>
-      <c r="J13" s="131"/>
-      <c r="K13" s="131"/>
-      <c r="L13" s="131"/>
-      <c r="M13" s="131"/>
-      <c r="N13" s="131"/>
-      <c r="O13" s="131"/>
-      <c r="P13" s="131"/>
-      <c r="Q13" s="131"/>
-      <c r="R13" s="131"/>
-      <c r="S13" s="131"/>
-      <c r="T13" s="131"/>
-      <c r="U13" s="133"/>
-      <c r="V13" s="133"/>
-      <c r="W13" s="131"/>
-      <c r="X13" s="131"/>
-      <c r="Y13" s="131"/>
-      <c r="Z13" s="131"/>
-      <c r="AA13" s="131"/>
-      <c r="AB13" s="131"/>
-      <c r="AC13" s="131"/>
-      <c r="AD13" s="131"/>
-      <c r="AE13" s="131"/>
-      <c r="AF13" s="131"/>
-      <c r="AG13" s="131"/>
-      <c r="AH13" s="131"/>
-      <c r="AI13" s="131"/>
-      <c r="AJ13" s="131"/>
-      <c r="AK13" s="131"/>
-      <c r="AL13" s="131"/>
-      <c r="AM13" s="131"/>
-      <c r="AN13" s="131"/>
-      <c r="AO13" s="131"/>
-      <c r="AP13" s="131"/>
-      <c r="AQ13" s="131"/>
-      <c r="AR13" s="131"/>
-      <c r="AS13" s="131"/>
-      <c r="AT13" s="131"/>
-      <c r="AU13" s="131"/>
-      <c r="AV13" s="131"/>
-      <c r="AW13" s="131"/>
-      <c r="AX13" s="131"/>
-      <c r="AY13" s="131"/>
-      <c r="AZ13" s="131"/>
-      <c r="BA13" s="131"/>
-      <c r="BB13" s="131"/>
-      <c r="BC13" s="131"/>
-      <c r="BD13" s="131"/>
-      <c r="BE13" s="131"/>
-      <c r="BF13" s="131"/>
-      <c r="BG13" s="131"/>
-      <c r="BH13" s="131"/>
-      <c r="BI13" s="131"/>
-      <c r="BJ13" s="131"/>
-      <c r="BK13" s="131"/>
-      <c r="BL13" s="131"/>
+      <c r="I13" s="130"/>
+      <c r="J13" s="130"/>
+      <c r="K13" s="130"/>
+      <c r="L13" s="130"/>
+      <c r="M13" s="130"/>
+      <c r="N13" s="130"/>
+      <c r="O13" s="130"/>
+      <c r="P13" s="130"/>
+      <c r="Q13" s="130"/>
+      <c r="R13" s="130"/>
+      <c r="S13" s="130"/>
+      <c r="T13" s="130"/>
+      <c r="U13" s="132"/>
+      <c r="V13" s="132"/>
+      <c r="W13" s="130"/>
+      <c r="X13" s="130"/>
+      <c r="Y13" s="130"/>
+      <c r="Z13" s="130"/>
+      <c r="AA13" s="130"/>
+      <c r="AB13" s="130"/>
+      <c r="AC13" s="130"/>
+      <c r="AD13" s="130"/>
+      <c r="AE13" s="130"/>
+      <c r="AF13" s="130"/>
+      <c r="AG13" s="130"/>
+      <c r="AH13" s="130"/>
+      <c r="AI13" s="130"/>
+      <c r="AJ13" s="130"/>
+      <c r="AK13" s="130"/>
+      <c r="AL13" s="130"/>
+      <c r="AM13" s="130"/>
+      <c r="AN13" s="130"/>
+      <c r="AO13" s="130"/>
+      <c r="AP13" s="130"/>
+      <c r="AQ13" s="130"/>
+      <c r="AR13" s="130"/>
+      <c r="AS13" s="130"/>
+      <c r="AT13" s="130"/>
+      <c r="AU13" s="130"/>
+      <c r="AV13" s="130"/>
+      <c r="AW13" s="130"/>
+      <c r="AX13" s="130"/>
+      <c r="AY13" s="130"/>
+      <c r="AZ13" s="130"/>
+      <c r="BA13" s="130"/>
+      <c r="BB13" s="130"/>
+      <c r="BC13" s="130"/>
+      <c r="BD13" s="130"/>
+      <c r="BE13" s="130"/>
+      <c r="BF13" s="130"/>
+      <c r="BG13" s="130"/>
+      <c r="BH13" s="130"/>
+      <c r="BI13" s="130"/>
+      <c r="BJ13" s="130"/>
+      <c r="BK13" s="130"/>
+      <c r="BL13" s="130"/>
     </row>
     <row r="14" s="50" customFormat="1" customHeight="1" spans="1:64">
       <c r="A14" s="51"/>
@@ -3542,62 +3536,62 @@
         <f>IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
         <v>2</v>
       </c>
-      <c r="I14" s="131"/>
-      <c r="J14" s="131"/>
-      <c r="K14" s="131"/>
-      <c r="L14" s="131"/>
-      <c r="M14" s="131"/>
-      <c r="N14" s="131"/>
-      <c r="O14" s="131"/>
-      <c r="P14" s="131"/>
-      <c r="Q14" s="131"/>
-      <c r="R14" s="131"/>
-      <c r="S14" s="131"/>
-      <c r="T14" s="131"/>
-      <c r="U14" s="131"/>
-      <c r="V14" s="131"/>
-      <c r="W14" s="131"/>
-      <c r="X14" s="131"/>
-      <c r="Y14" s="131"/>
-      <c r="Z14" s="131"/>
-      <c r="AA14" s="131"/>
-      <c r="AB14" s="131"/>
-      <c r="AC14" s="131"/>
-      <c r="AD14" s="131"/>
-      <c r="AE14" s="131"/>
-      <c r="AF14" s="131"/>
-      <c r="AG14" s="131"/>
-      <c r="AH14" s="131"/>
-      <c r="AI14" s="131"/>
-      <c r="AJ14" s="131"/>
-      <c r="AK14" s="131"/>
-      <c r="AL14" s="131"/>
-      <c r="AM14" s="131"/>
-      <c r="AN14" s="131"/>
-      <c r="AO14" s="131"/>
-      <c r="AP14" s="131"/>
-      <c r="AQ14" s="131"/>
-      <c r="AR14" s="131"/>
-      <c r="AS14" s="131"/>
-      <c r="AT14" s="131"/>
-      <c r="AU14" s="131"/>
-      <c r="AV14" s="131"/>
-      <c r="AW14" s="131"/>
-      <c r="AX14" s="131"/>
-      <c r="AY14" s="131"/>
-      <c r="AZ14" s="131"/>
-      <c r="BA14" s="131"/>
-      <c r="BB14" s="131"/>
-      <c r="BC14" s="131"/>
-      <c r="BD14" s="131"/>
-      <c r="BE14" s="131"/>
-      <c r="BF14" s="131"/>
-      <c r="BG14" s="131"/>
-      <c r="BH14" s="131"/>
-      <c r="BI14" s="131"/>
-      <c r="BJ14" s="131"/>
-      <c r="BK14" s="131"/>
-      <c r="BL14" s="131"/>
+      <c r="I14" s="130"/>
+      <c r="J14" s="130"/>
+      <c r="K14" s="130"/>
+      <c r="L14" s="130"/>
+      <c r="M14" s="130"/>
+      <c r="N14" s="130"/>
+      <c r="O14" s="130"/>
+      <c r="P14" s="130"/>
+      <c r="Q14" s="130"/>
+      <c r="R14" s="130"/>
+      <c r="S14" s="130"/>
+      <c r="T14" s="130"/>
+      <c r="U14" s="130"/>
+      <c r="V14" s="130"/>
+      <c r="W14" s="130"/>
+      <c r="X14" s="130"/>
+      <c r="Y14" s="130"/>
+      <c r="Z14" s="130"/>
+      <c r="AA14" s="130"/>
+      <c r="AB14" s="130"/>
+      <c r="AC14" s="130"/>
+      <c r="AD14" s="130"/>
+      <c r="AE14" s="130"/>
+      <c r="AF14" s="130"/>
+      <c r="AG14" s="130"/>
+      <c r="AH14" s="130"/>
+      <c r="AI14" s="130"/>
+      <c r="AJ14" s="130"/>
+      <c r="AK14" s="130"/>
+      <c r="AL14" s="130"/>
+      <c r="AM14" s="130"/>
+      <c r="AN14" s="130"/>
+      <c r="AO14" s="130"/>
+      <c r="AP14" s="130"/>
+      <c r="AQ14" s="130"/>
+      <c r="AR14" s="130"/>
+      <c r="AS14" s="130"/>
+      <c r="AT14" s="130"/>
+      <c r="AU14" s="130"/>
+      <c r="AV14" s="130"/>
+      <c r="AW14" s="130"/>
+      <c r="AX14" s="130"/>
+      <c r="AY14" s="130"/>
+      <c r="AZ14" s="130"/>
+      <c r="BA14" s="130"/>
+      <c r="BB14" s="130"/>
+      <c r="BC14" s="130"/>
+      <c r="BD14" s="130"/>
+      <c r="BE14" s="130"/>
+      <c r="BF14" s="130"/>
+      <c r="BG14" s="130"/>
+      <c r="BH14" s="130"/>
+      <c r="BI14" s="130"/>
+      <c r="BJ14" s="130"/>
+      <c r="BK14" s="130"/>
+      <c r="BL14" s="130"/>
     </row>
     <row r="15" s="50" customFormat="1" customHeight="1" spans="1:64">
       <c r="A15" s="51"/>
@@ -3621,910 +3615,954 @@
         <f>IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
         <v>2</v>
       </c>
-      <c r="I15" s="131"/>
-      <c r="J15" s="131"/>
-      <c r="K15" s="131"/>
-      <c r="L15" s="131"/>
-      <c r="M15" s="131"/>
-      <c r="N15" s="131"/>
-      <c r="O15" s="131"/>
-      <c r="P15" s="131"/>
-      <c r="Q15" s="131"/>
-      <c r="R15" s="131"/>
-      <c r="S15" s="131"/>
-      <c r="T15" s="131"/>
-      <c r="U15" s="131"/>
-      <c r="V15" s="131"/>
-      <c r="W15" s="131"/>
-      <c r="X15" s="131"/>
-      <c r="Y15" s="133"/>
-      <c r="Z15" s="131"/>
-      <c r="AA15" s="131"/>
-      <c r="AB15" s="131"/>
-      <c r="AC15" s="131"/>
-      <c r="AD15" s="131"/>
-      <c r="AE15" s="131"/>
-      <c r="AF15" s="131"/>
-      <c r="AG15" s="131"/>
-      <c r="AH15" s="131"/>
-      <c r="AI15" s="131"/>
-      <c r="AJ15" s="131"/>
-      <c r="AK15" s="131"/>
-      <c r="AL15" s="131"/>
-      <c r="AM15" s="131"/>
-      <c r="AN15" s="131"/>
-      <c r="AO15" s="131"/>
-      <c r="AP15" s="131"/>
-      <c r="AQ15" s="131"/>
-      <c r="AR15" s="131"/>
-      <c r="AS15" s="131"/>
-      <c r="AT15" s="131"/>
-      <c r="AU15" s="131"/>
-      <c r="AV15" s="131"/>
-      <c r="AW15" s="131"/>
-      <c r="AX15" s="131"/>
-      <c r="AY15" s="131"/>
-      <c r="AZ15" s="131"/>
-      <c r="BA15" s="131"/>
-      <c r="BB15" s="131"/>
-      <c r="BC15" s="131"/>
-      <c r="BD15" s="131"/>
-      <c r="BE15" s="131"/>
-      <c r="BF15" s="131"/>
-      <c r="BG15" s="131"/>
-      <c r="BH15" s="131"/>
-      <c r="BI15" s="131"/>
-      <c r="BJ15" s="131"/>
-      <c r="BK15" s="131"/>
-      <c r="BL15" s="131"/>
+      <c r="I15" s="130"/>
+      <c r="J15" s="130"/>
+      <c r="K15" s="130"/>
+      <c r="L15" s="130"/>
+      <c r="M15" s="130"/>
+      <c r="N15" s="130"/>
+      <c r="O15" s="130"/>
+      <c r="P15" s="130"/>
+      <c r="Q15" s="130"/>
+      <c r="R15" s="130"/>
+      <c r="S15" s="130"/>
+      <c r="T15" s="130"/>
+      <c r="U15" s="130"/>
+      <c r="V15" s="130"/>
+      <c r="W15" s="130"/>
+      <c r="X15" s="130"/>
+      <c r="Y15" s="132"/>
+      <c r="Z15" s="130"/>
+      <c r="AA15" s="130"/>
+      <c r="AB15" s="130"/>
+      <c r="AC15" s="130"/>
+      <c r="AD15" s="130"/>
+      <c r="AE15" s="130"/>
+      <c r="AF15" s="130"/>
+      <c r="AG15" s="130"/>
+      <c r="AH15" s="130"/>
+      <c r="AI15" s="130"/>
+      <c r="AJ15" s="130"/>
+      <c r="AK15" s="130"/>
+      <c r="AL15" s="130"/>
+      <c r="AM15" s="130"/>
+      <c r="AN15" s="130"/>
+      <c r="AO15" s="130"/>
+      <c r="AP15" s="130"/>
+      <c r="AQ15" s="130"/>
+      <c r="AR15" s="130"/>
+      <c r="AS15" s="130"/>
+      <c r="AT15" s="130"/>
+      <c r="AU15" s="130"/>
+      <c r="AV15" s="130"/>
+      <c r="AW15" s="130"/>
+      <c r="AX15" s="130"/>
+      <c r="AY15" s="130"/>
+      <c r="AZ15" s="130"/>
+      <c r="BA15" s="130"/>
+      <c r="BB15" s="130"/>
+      <c r="BC15" s="130"/>
+      <c r="BD15" s="130"/>
+      <c r="BE15" s="130"/>
+      <c r="BF15" s="130"/>
+      <c r="BG15" s="130"/>
+      <c r="BH15" s="130"/>
+      <c r="BI15" s="130"/>
+      <c r="BJ15" s="130"/>
+      <c r="BK15" s="130"/>
+      <c r="BL15" s="130"/>
     </row>
     <row r="16" s="50" customFormat="1" customHeight="1" spans="1:64">
       <c r="A16" s="51" t="s">
         <v>33</v>
       </c>
-      <c r="B16" s="90" t="s">
+      <c r="B16" s="89" t="s">
         <v>34</v>
       </c>
-      <c r="C16" s="91"/>
-      <c r="D16" s="92"/>
-      <c r="E16" s="93"/>
-      <c r="F16" s="94"/>
+      <c r="C16" s="90"/>
+      <c r="D16" s="91"/>
+      <c r="E16" s="92"/>
+      <c r="F16" s="93"/>
       <c r="G16" s="74"/>
       <c r="H16" s="74" t="str">
-        <f t="shared" ref="H16:H29" si="6">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
+        <f>IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
         <v/>
       </c>
-      <c r="I16" s="131"/>
-      <c r="J16" s="131"/>
-      <c r="K16" s="131"/>
-      <c r="L16" s="131"/>
-      <c r="M16" s="131"/>
-      <c r="N16" s="131"/>
-      <c r="O16" s="131"/>
-      <c r="P16" s="131"/>
-      <c r="Q16" s="131"/>
-      <c r="R16" s="131"/>
-      <c r="S16" s="131"/>
-      <c r="T16" s="131"/>
-      <c r="U16" s="131"/>
-      <c r="V16" s="131"/>
-      <c r="W16" s="131"/>
-      <c r="X16" s="131"/>
-      <c r="Y16" s="131"/>
-      <c r="Z16" s="131"/>
-      <c r="AA16" s="131"/>
-      <c r="AB16" s="131"/>
-      <c r="AC16" s="131"/>
-      <c r="AD16" s="131"/>
-      <c r="AE16" s="131"/>
-      <c r="AF16" s="131"/>
-      <c r="AG16" s="131"/>
-      <c r="AH16" s="131"/>
-      <c r="AI16" s="131"/>
-      <c r="AJ16" s="131"/>
-      <c r="AK16" s="131"/>
-      <c r="AL16" s="131"/>
-      <c r="AM16" s="131"/>
-      <c r="AN16" s="131"/>
-      <c r="AO16" s="131"/>
-      <c r="AP16" s="131"/>
-      <c r="AQ16" s="131"/>
-      <c r="AR16" s="131"/>
-      <c r="AS16" s="131"/>
-      <c r="AT16" s="131"/>
-      <c r="AU16" s="131"/>
-      <c r="AV16" s="131"/>
-      <c r="AW16" s="131"/>
-      <c r="AX16" s="131"/>
-      <c r="AY16" s="131"/>
-      <c r="AZ16" s="131"/>
-      <c r="BA16" s="131"/>
-      <c r="BB16" s="131"/>
-      <c r="BC16" s="131"/>
-      <c r="BD16" s="131"/>
-      <c r="BE16" s="131"/>
-      <c r="BF16" s="131"/>
-      <c r="BG16" s="131"/>
-      <c r="BH16" s="131"/>
-      <c r="BI16" s="131"/>
-      <c r="BJ16" s="131"/>
-      <c r="BK16" s="131"/>
-      <c r="BL16" s="131"/>
+      <c r="I16" s="130"/>
+      <c r="J16" s="130"/>
+      <c r="K16" s="130"/>
+      <c r="L16" s="130"/>
+      <c r="M16" s="130"/>
+      <c r="N16" s="130"/>
+      <c r="O16" s="130"/>
+      <c r="P16" s="130"/>
+      <c r="Q16" s="130"/>
+      <c r="R16" s="130"/>
+      <c r="S16" s="130"/>
+      <c r="T16" s="130"/>
+      <c r="U16" s="130"/>
+      <c r="V16" s="130"/>
+      <c r="W16" s="130"/>
+      <c r="X16" s="130"/>
+      <c r="Y16" s="130"/>
+      <c r="Z16" s="130"/>
+      <c r="AA16" s="130"/>
+      <c r="AB16" s="130"/>
+      <c r="AC16" s="130"/>
+      <c r="AD16" s="130"/>
+      <c r="AE16" s="130"/>
+      <c r="AF16" s="130"/>
+      <c r="AG16" s="130"/>
+      <c r="AH16" s="130"/>
+      <c r="AI16" s="130"/>
+      <c r="AJ16" s="130"/>
+      <c r="AK16" s="130"/>
+      <c r="AL16" s="130"/>
+      <c r="AM16" s="130"/>
+      <c r="AN16" s="130"/>
+      <c r="AO16" s="130"/>
+      <c r="AP16" s="130"/>
+      <c r="AQ16" s="130"/>
+      <c r="AR16" s="130"/>
+      <c r="AS16" s="130"/>
+      <c r="AT16" s="130"/>
+      <c r="AU16" s="130"/>
+      <c r="AV16" s="130"/>
+      <c r="AW16" s="130"/>
+      <c r="AX16" s="130"/>
+      <c r="AY16" s="130"/>
+      <c r="AZ16" s="130"/>
+      <c r="BA16" s="130"/>
+      <c r="BB16" s="130"/>
+      <c r="BC16" s="130"/>
+      <c r="BD16" s="130"/>
+      <c r="BE16" s="130"/>
+      <c r="BF16" s="130"/>
+      <c r="BG16" s="130"/>
+      <c r="BH16" s="130"/>
+      <c r="BI16" s="130"/>
+      <c r="BJ16" s="130"/>
+      <c r="BK16" s="130"/>
+      <c r="BL16" s="130"/>
     </row>
     <row r="17" s="50" customFormat="1" customHeight="1" spans="1:64">
       <c r="A17" s="51"/>
-      <c r="B17" s="95"/>
-      <c r="C17" s="96"/>
-      <c r="D17" s="97"/>
-      <c r="E17" s="98"/>
-      <c r="F17" s="98"/>
+      <c r="B17" s="94" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" s="95"/>
+      <c r="D17" s="96">
+        <v>0.5</v>
+      </c>
+      <c r="E17" s="97">
+        <f>F15</f>
+        <v>45083</v>
+      </c>
+      <c r="F17" s="97">
+        <f>E17+1</f>
+        <v>45084</v>
+      </c>
       <c r="G17" s="74"/>
-      <c r="H17" s="74" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="I17" s="131"/>
-      <c r="J17" s="131"/>
-      <c r="K17" s="131"/>
-      <c r="L17" s="131"/>
-      <c r="M17" s="131"/>
-      <c r="N17" s="131"/>
-      <c r="O17" s="131"/>
-      <c r="P17" s="131"/>
-      <c r="Q17" s="131"/>
-      <c r="R17" s="131"/>
-      <c r="S17" s="131"/>
-      <c r="T17" s="131"/>
-      <c r="U17" s="131"/>
-      <c r="V17" s="131"/>
-      <c r="W17" s="131"/>
-      <c r="X17" s="131"/>
-      <c r="Y17" s="131"/>
-      <c r="Z17" s="131"/>
-      <c r="AA17" s="131"/>
-      <c r="AB17" s="131"/>
-      <c r="AC17" s="131"/>
-      <c r="AD17" s="131"/>
-      <c r="AE17" s="131"/>
-      <c r="AF17" s="131"/>
-      <c r="AG17" s="131"/>
-      <c r="AH17" s="131"/>
-      <c r="AI17" s="131"/>
-      <c r="AJ17" s="131"/>
-      <c r="AK17" s="131"/>
-      <c r="AL17" s="131"/>
-      <c r="AM17" s="131"/>
-      <c r="AN17" s="131"/>
-      <c r="AO17" s="131"/>
-      <c r="AP17" s="131"/>
-      <c r="AQ17" s="131"/>
-      <c r="AR17" s="131"/>
-      <c r="AS17" s="131"/>
-      <c r="AT17" s="131"/>
-      <c r="AU17" s="131"/>
-      <c r="AV17" s="131"/>
-      <c r="AW17" s="131"/>
-      <c r="AX17" s="131"/>
-      <c r="AY17" s="131"/>
-      <c r="AZ17" s="131"/>
-      <c r="BA17" s="131"/>
-      <c r="BB17" s="131"/>
-      <c r="BC17" s="131"/>
-      <c r="BD17" s="131"/>
-      <c r="BE17" s="131"/>
-      <c r="BF17" s="131"/>
-      <c r="BG17" s="131"/>
-      <c r="BH17" s="131"/>
-      <c r="BI17" s="131"/>
-      <c r="BJ17" s="131"/>
-      <c r="BK17" s="131"/>
-      <c r="BL17" s="131"/>
+      <c r="H17" s="74">
+        <f>IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
+        <v>2</v>
+      </c>
+      <c r="I17" s="130"/>
+      <c r="J17" s="130"/>
+      <c r="K17" s="130"/>
+      <c r="L17" s="130"/>
+      <c r="M17" s="130"/>
+      <c r="N17" s="130"/>
+      <c r="O17" s="130"/>
+      <c r="P17" s="130"/>
+      <c r="Q17" s="130"/>
+      <c r="R17" s="130"/>
+      <c r="S17" s="130"/>
+      <c r="T17" s="130"/>
+      <c r="U17" s="130"/>
+      <c r="V17" s="130"/>
+      <c r="W17" s="130"/>
+      <c r="X17" s="130"/>
+      <c r="Y17" s="130"/>
+      <c r="Z17" s="130"/>
+      <c r="AA17" s="130"/>
+      <c r="AB17" s="130"/>
+      <c r="AC17" s="130"/>
+      <c r="AD17" s="130"/>
+      <c r="AE17" s="130"/>
+      <c r="AF17" s="130"/>
+      <c r="AG17" s="130"/>
+      <c r="AH17" s="130"/>
+      <c r="AI17" s="130"/>
+      <c r="AJ17" s="130"/>
+      <c r="AK17" s="130"/>
+      <c r="AL17" s="130"/>
+      <c r="AM17" s="130"/>
+      <c r="AN17" s="130"/>
+      <c r="AO17" s="130"/>
+      <c r="AP17" s="130"/>
+      <c r="AQ17" s="130"/>
+      <c r="AR17" s="130"/>
+      <c r="AS17" s="130"/>
+      <c r="AT17" s="130"/>
+      <c r="AU17" s="130"/>
+      <c r="AV17" s="130"/>
+      <c r="AW17" s="130"/>
+      <c r="AX17" s="130"/>
+      <c r="AY17" s="130"/>
+      <c r="AZ17" s="130"/>
+      <c r="BA17" s="130"/>
+      <c r="BB17" s="130"/>
+      <c r="BC17" s="130"/>
+      <c r="BD17" s="130"/>
+      <c r="BE17" s="130"/>
+      <c r="BF17" s="130"/>
+      <c r="BG17" s="130"/>
+      <c r="BH17" s="130"/>
+      <c r="BI17" s="130"/>
+      <c r="BJ17" s="130"/>
+      <c r="BK17" s="130"/>
+      <c r="BL17" s="130"/>
     </row>
     <row r="18" s="50" customFormat="1" customHeight="1" spans="1:64">
       <c r="A18" s="51"/>
-      <c r="B18" s="95"/>
-      <c r="C18" s="96"/>
-      <c r="D18" s="97"/>
-      <c r="E18" s="98"/>
-      <c r="F18" s="98"/>
+      <c r="B18" s="94" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" s="95"/>
+      <c r="D18" s="96">
+        <v>0</v>
+      </c>
+      <c r="E18" s="97">
+        <f>F17+1</f>
+        <v>45085</v>
+      </c>
+      <c r="F18" s="97">
+        <f>E18+1</f>
+        <v>45086</v>
+      </c>
       <c r="G18" s="74"/>
-      <c r="H18" s="74" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="I18" s="131"/>
-      <c r="J18" s="131"/>
-      <c r="K18" s="131"/>
-      <c r="L18" s="131"/>
-      <c r="M18" s="131"/>
-      <c r="N18" s="131"/>
-      <c r="O18" s="131"/>
-      <c r="P18" s="131"/>
-      <c r="Q18" s="131"/>
-      <c r="R18" s="131"/>
-      <c r="S18" s="131"/>
-      <c r="T18" s="131"/>
-      <c r="U18" s="131"/>
-      <c r="V18" s="131"/>
-      <c r="W18" s="131"/>
-      <c r="X18" s="131"/>
-      <c r="Y18" s="131"/>
-      <c r="Z18" s="131"/>
-      <c r="AA18" s="131"/>
-      <c r="AB18" s="131"/>
-      <c r="AC18" s="131"/>
-      <c r="AD18" s="131"/>
-      <c r="AE18" s="131"/>
-      <c r="AF18" s="131"/>
-      <c r="AG18" s="131"/>
-      <c r="AH18" s="131"/>
-      <c r="AI18" s="131"/>
-      <c r="AJ18" s="131"/>
-      <c r="AK18" s="131"/>
-      <c r="AL18" s="131"/>
-      <c r="AM18" s="131"/>
-      <c r="AN18" s="131"/>
-      <c r="AO18" s="131"/>
-      <c r="AP18" s="131"/>
-      <c r="AQ18" s="131"/>
-      <c r="AR18" s="131"/>
-      <c r="AS18" s="131"/>
-      <c r="AT18" s="131"/>
-      <c r="AU18" s="131"/>
-      <c r="AV18" s="131"/>
-      <c r="AW18" s="131"/>
-      <c r="AX18" s="131"/>
-      <c r="AY18" s="131"/>
-      <c r="AZ18" s="131"/>
-      <c r="BA18" s="131"/>
-      <c r="BB18" s="131"/>
-      <c r="BC18" s="131"/>
-      <c r="BD18" s="131"/>
-      <c r="BE18" s="131"/>
-      <c r="BF18" s="131"/>
-      <c r="BG18" s="131"/>
-      <c r="BH18" s="131"/>
-      <c r="BI18" s="131"/>
-      <c r="BJ18" s="131"/>
-      <c r="BK18" s="131"/>
-      <c r="BL18" s="131"/>
+      <c r="H18" s="74">
+        <f>IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
+        <v>2</v>
+      </c>
+      <c r="I18" s="130"/>
+      <c r="J18" s="130"/>
+      <c r="K18" s="130"/>
+      <c r="L18" s="130"/>
+      <c r="M18" s="130"/>
+      <c r="N18" s="130"/>
+      <c r="O18" s="130"/>
+      <c r="P18" s="130"/>
+      <c r="Q18" s="130"/>
+      <c r="R18" s="130"/>
+      <c r="S18" s="130"/>
+      <c r="T18" s="130"/>
+      <c r="U18" s="130"/>
+      <c r="V18" s="130"/>
+      <c r="W18" s="130"/>
+      <c r="X18" s="130"/>
+      <c r="Y18" s="130"/>
+      <c r="Z18" s="130"/>
+      <c r="AA18" s="130"/>
+      <c r="AB18" s="130"/>
+      <c r="AC18" s="130"/>
+      <c r="AD18" s="130"/>
+      <c r="AE18" s="130"/>
+      <c r="AF18" s="130"/>
+      <c r="AG18" s="130"/>
+      <c r="AH18" s="130"/>
+      <c r="AI18" s="130"/>
+      <c r="AJ18" s="130"/>
+      <c r="AK18" s="130"/>
+      <c r="AL18" s="130"/>
+      <c r="AM18" s="130"/>
+      <c r="AN18" s="130"/>
+      <c r="AO18" s="130"/>
+      <c r="AP18" s="130"/>
+      <c r="AQ18" s="130"/>
+      <c r="AR18" s="130"/>
+      <c r="AS18" s="130"/>
+      <c r="AT18" s="130"/>
+      <c r="AU18" s="130"/>
+      <c r="AV18" s="130"/>
+      <c r="AW18" s="130"/>
+      <c r="AX18" s="130"/>
+      <c r="AY18" s="130"/>
+      <c r="AZ18" s="130"/>
+      <c r="BA18" s="130"/>
+      <c r="BB18" s="130"/>
+      <c r="BC18" s="130"/>
+      <c r="BD18" s="130"/>
+      <c r="BE18" s="130"/>
+      <c r="BF18" s="130"/>
+      <c r="BG18" s="130"/>
+      <c r="BH18" s="130"/>
+      <c r="BI18" s="130"/>
+      <c r="BJ18" s="130"/>
+      <c r="BK18" s="130"/>
+      <c r="BL18" s="130"/>
     </row>
     <row r="19" s="50" customFormat="1" customHeight="1" spans="1:64">
       <c r="A19" s="51"/>
-      <c r="B19" s="95"/>
-      <c r="C19" s="96"/>
-      <c r="D19" s="97"/>
-      <c r="E19" s="98"/>
-      <c r="F19" s="98"/>
+      <c r="B19" s="94" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" s="95"/>
+      <c r="D19" s="96">
+        <v>0</v>
+      </c>
+      <c r="E19" s="97">
+        <f>F18+1</f>
+        <v>45087</v>
+      </c>
+      <c r="F19" s="97">
+        <f>E19+1</f>
+        <v>45088</v>
+      </c>
       <c r="G19" s="74"/>
-      <c r="H19" s="74" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="I19" s="131"/>
-      <c r="J19" s="131"/>
-      <c r="K19" s="131"/>
-      <c r="L19" s="131"/>
-      <c r="M19" s="131"/>
-      <c r="N19" s="131"/>
-      <c r="O19" s="131"/>
-      <c r="P19" s="131"/>
-      <c r="Q19" s="131"/>
-      <c r="R19" s="131"/>
-      <c r="S19" s="131"/>
-      <c r="T19" s="131"/>
-      <c r="U19" s="131"/>
-      <c r="V19" s="131"/>
-      <c r="W19" s="131"/>
-      <c r="X19" s="131"/>
-      <c r="Y19" s="131"/>
-      <c r="Z19" s="131"/>
-      <c r="AA19" s="131"/>
-      <c r="AB19" s="131"/>
-      <c r="AC19" s="131"/>
-      <c r="AD19" s="131"/>
-      <c r="AE19" s="131"/>
-      <c r="AF19" s="131"/>
-      <c r="AG19" s="131"/>
-      <c r="AH19" s="131"/>
-      <c r="AI19" s="131"/>
-      <c r="AJ19" s="131"/>
-      <c r="AK19" s="131"/>
-      <c r="AL19" s="131"/>
-      <c r="AM19" s="131"/>
-      <c r="AN19" s="131"/>
-      <c r="AO19" s="131"/>
-      <c r="AP19" s="131"/>
-      <c r="AQ19" s="131"/>
-      <c r="AR19" s="131"/>
-      <c r="AS19" s="131"/>
-      <c r="AT19" s="131"/>
-      <c r="AU19" s="131"/>
-      <c r="AV19" s="131"/>
-      <c r="AW19" s="131"/>
-      <c r="AX19" s="131"/>
-      <c r="AY19" s="131"/>
-      <c r="AZ19" s="131"/>
-      <c r="BA19" s="131"/>
-      <c r="BB19" s="131"/>
-      <c r="BC19" s="131"/>
-      <c r="BD19" s="131"/>
-      <c r="BE19" s="131"/>
-      <c r="BF19" s="131"/>
-      <c r="BG19" s="131"/>
-      <c r="BH19" s="131"/>
-      <c r="BI19" s="131"/>
-      <c r="BJ19" s="131"/>
-      <c r="BK19" s="131"/>
-      <c r="BL19" s="131"/>
+      <c r="H19" s="74">
+        <f>IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
+        <v>2</v>
+      </c>
+      <c r="I19" s="130"/>
+      <c r="J19" s="130"/>
+      <c r="K19" s="130"/>
+      <c r="L19" s="130"/>
+      <c r="M19" s="130"/>
+      <c r="N19" s="130"/>
+      <c r="O19" s="130"/>
+      <c r="P19" s="130"/>
+      <c r="Q19" s="130"/>
+      <c r="R19" s="130"/>
+      <c r="S19" s="130"/>
+      <c r="T19" s="130"/>
+      <c r="U19" s="130"/>
+      <c r="V19" s="130"/>
+      <c r="W19" s="130"/>
+      <c r="X19" s="130"/>
+      <c r="Y19" s="130"/>
+      <c r="Z19" s="130"/>
+      <c r="AA19" s="130"/>
+      <c r="AB19" s="130"/>
+      <c r="AC19" s="130"/>
+      <c r="AD19" s="130"/>
+      <c r="AE19" s="130"/>
+      <c r="AF19" s="130"/>
+      <c r="AG19" s="130"/>
+      <c r="AH19" s="130"/>
+      <c r="AI19" s="130"/>
+      <c r="AJ19" s="130"/>
+      <c r="AK19" s="130"/>
+      <c r="AL19" s="130"/>
+      <c r="AM19" s="130"/>
+      <c r="AN19" s="130"/>
+      <c r="AO19" s="130"/>
+      <c r="AP19" s="130"/>
+      <c r="AQ19" s="130"/>
+      <c r="AR19" s="130"/>
+      <c r="AS19" s="130"/>
+      <c r="AT19" s="130"/>
+      <c r="AU19" s="130"/>
+      <c r="AV19" s="130"/>
+      <c r="AW19" s="130"/>
+      <c r="AX19" s="130"/>
+      <c r="AY19" s="130"/>
+      <c r="AZ19" s="130"/>
+      <c r="BA19" s="130"/>
+      <c r="BB19" s="130"/>
+      <c r="BC19" s="130"/>
+      <c r="BD19" s="130"/>
+      <c r="BE19" s="130"/>
+      <c r="BF19" s="130"/>
+      <c r="BG19" s="130"/>
+      <c r="BH19" s="130"/>
+      <c r="BI19" s="130"/>
+      <c r="BJ19" s="130"/>
+      <c r="BK19" s="130"/>
+      <c r="BL19" s="130"/>
     </row>
     <row r="20" s="50" customFormat="1" customHeight="1" spans="1:64">
       <c r="A20" s="51"/>
-      <c r="B20" s="95"/>
-      <c r="C20" s="96"/>
-      <c r="D20" s="97"/>
-      <c r="E20" s="98"/>
-      <c r="F20" s="98"/>
+      <c r="B20" s="94" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" s="95"/>
+      <c r="D20" s="96">
+        <v>0</v>
+      </c>
+      <c r="E20" s="97">
+        <f>F19+1</f>
+        <v>45089</v>
+      </c>
+      <c r="F20" s="97">
+        <f>E20+3</f>
+        <v>45092</v>
+      </c>
       <c r="G20" s="74"/>
-      <c r="H20" s="74" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="I20" s="131"/>
-      <c r="J20" s="131"/>
-      <c r="K20" s="131"/>
-      <c r="L20" s="131"/>
-      <c r="M20" s="131"/>
-      <c r="N20" s="131"/>
-      <c r="O20" s="131"/>
-      <c r="P20" s="131"/>
-      <c r="Q20" s="131"/>
-      <c r="R20" s="131"/>
-      <c r="S20" s="131"/>
-      <c r="T20" s="131"/>
-      <c r="U20" s="131"/>
-      <c r="V20" s="131"/>
-      <c r="W20" s="131"/>
-      <c r="X20" s="131"/>
-      <c r="Y20" s="131"/>
-      <c r="Z20" s="131"/>
-      <c r="AA20" s="131"/>
-      <c r="AB20" s="131"/>
-      <c r="AC20" s="131"/>
-      <c r="AD20" s="131"/>
-      <c r="AE20" s="131"/>
-      <c r="AF20" s="131"/>
-      <c r="AG20" s="131"/>
-      <c r="AH20" s="131"/>
-      <c r="AI20" s="131"/>
-      <c r="AJ20" s="131"/>
-      <c r="AK20" s="131"/>
-      <c r="AL20" s="131"/>
-      <c r="AM20" s="131"/>
-      <c r="AN20" s="131"/>
-      <c r="AO20" s="131"/>
-      <c r="AP20" s="131"/>
-      <c r="AQ20" s="131"/>
-      <c r="AR20" s="131"/>
-      <c r="AS20" s="131"/>
-      <c r="AT20" s="131"/>
-      <c r="AU20" s="131"/>
-      <c r="AV20" s="131"/>
-      <c r="AW20" s="131"/>
-      <c r="AX20" s="131"/>
-      <c r="AY20" s="131"/>
-      <c r="AZ20" s="131"/>
-      <c r="BA20" s="131"/>
-      <c r="BB20" s="131"/>
-      <c r="BC20" s="131"/>
-      <c r="BD20" s="131"/>
-      <c r="BE20" s="131"/>
-      <c r="BF20" s="131"/>
-      <c r="BG20" s="131"/>
-      <c r="BH20" s="131"/>
-      <c r="BI20" s="131"/>
-      <c r="BJ20" s="131"/>
-      <c r="BK20" s="131"/>
-      <c r="BL20" s="131"/>
+      <c r="H20" s="74">
+        <f>IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
+        <v>4</v>
+      </c>
+      <c r="I20" s="130"/>
+      <c r="J20" s="130"/>
+      <c r="K20" s="130"/>
+      <c r="L20" s="130"/>
+      <c r="M20" s="130"/>
+      <c r="N20" s="130"/>
+      <c r="O20" s="130"/>
+      <c r="P20" s="130"/>
+      <c r="Q20" s="130"/>
+      <c r="R20" s="130"/>
+      <c r="S20" s="130"/>
+      <c r="T20" s="130"/>
+      <c r="U20" s="130"/>
+      <c r="V20" s="130"/>
+      <c r="W20" s="130"/>
+      <c r="X20" s="130"/>
+      <c r="Y20" s="130"/>
+      <c r="Z20" s="130"/>
+      <c r="AA20" s="130"/>
+      <c r="AB20" s="130"/>
+      <c r="AC20" s="130"/>
+      <c r="AD20" s="130"/>
+      <c r="AE20" s="130"/>
+      <c r="AF20" s="130"/>
+      <c r="AG20" s="130"/>
+      <c r="AH20" s="130"/>
+      <c r="AI20" s="130"/>
+      <c r="AJ20" s="130"/>
+      <c r="AK20" s="130"/>
+      <c r="AL20" s="130"/>
+      <c r="AM20" s="130"/>
+      <c r="AN20" s="130"/>
+      <c r="AO20" s="130"/>
+      <c r="AP20" s="130"/>
+      <c r="AQ20" s="130"/>
+      <c r="AR20" s="130"/>
+      <c r="AS20" s="130"/>
+      <c r="AT20" s="130"/>
+      <c r="AU20" s="130"/>
+      <c r="AV20" s="130"/>
+      <c r="AW20" s="130"/>
+      <c r="AX20" s="130"/>
+      <c r="AY20" s="130"/>
+      <c r="AZ20" s="130"/>
+      <c r="BA20" s="130"/>
+      <c r="BB20" s="130"/>
+      <c r="BC20" s="130"/>
+      <c r="BD20" s="130"/>
+      <c r="BE20" s="130"/>
+      <c r="BF20" s="130"/>
+      <c r="BG20" s="130"/>
+      <c r="BH20" s="130"/>
+      <c r="BI20" s="130"/>
+      <c r="BJ20" s="130"/>
+      <c r="BK20" s="130"/>
+      <c r="BL20" s="130"/>
     </row>
     <row r="21" s="50" customFormat="1" customHeight="1" spans="1:64">
-      <c r="A21" s="51"/>
-      <c r="B21" s="95"/>
-      <c r="C21" s="96"/>
-      <c r="D21" s="97"/>
-      <c r="E21" s="98"/>
-      <c r="F21" s="98"/>
+      <c r="A21" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21" s="98" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21" s="99"/>
+      <c r="D21" s="100"/>
+      <c r="E21" s="101"/>
+      <c r="F21" s="102"/>
       <c r="G21" s="74"/>
       <c r="H21" s="74" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" ref="H21:H28" si="6">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
         <v/>
       </c>
-      <c r="I21" s="131"/>
-      <c r="J21" s="131"/>
-      <c r="K21" s="131"/>
-      <c r="L21" s="131"/>
-      <c r="M21" s="131"/>
-      <c r="N21" s="131"/>
-      <c r="O21" s="131"/>
-      <c r="P21" s="131"/>
-      <c r="Q21" s="131"/>
-      <c r="R21" s="131"/>
-      <c r="S21" s="131"/>
-      <c r="T21" s="131"/>
-      <c r="U21" s="131"/>
-      <c r="V21" s="131"/>
-      <c r="W21" s="131"/>
-      <c r="X21" s="131"/>
-      <c r="Y21" s="131"/>
-      <c r="Z21" s="131"/>
-      <c r="AA21" s="131"/>
-      <c r="AB21" s="131"/>
-      <c r="AC21" s="131"/>
-      <c r="AD21" s="131"/>
-      <c r="AE21" s="131"/>
-      <c r="AF21" s="131"/>
-      <c r="AG21" s="131"/>
-      <c r="AH21" s="131"/>
-      <c r="AI21" s="131"/>
-      <c r="AJ21" s="131"/>
-      <c r="AK21" s="131"/>
-      <c r="AL21" s="131"/>
-      <c r="AM21" s="131"/>
-      <c r="AN21" s="131"/>
-      <c r="AO21" s="131"/>
-      <c r="AP21" s="131"/>
-      <c r="AQ21" s="131"/>
-      <c r="AR21" s="131"/>
-      <c r="AS21" s="131"/>
-      <c r="AT21" s="131"/>
-      <c r="AU21" s="131"/>
-      <c r="AV21" s="131"/>
-      <c r="AW21" s="131"/>
-      <c r="AX21" s="131"/>
-      <c r="AY21" s="131"/>
-      <c r="AZ21" s="131"/>
-      <c r="BA21" s="131"/>
-      <c r="BB21" s="131"/>
-      <c r="BC21" s="131"/>
-      <c r="BD21" s="131"/>
-      <c r="BE21" s="131"/>
-      <c r="BF21" s="131"/>
-      <c r="BG21" s="131"/>
-      <c r="BH21" s="131"/>
-      <c r="BI21" s="131"/>
-      <c r="BJ21" s="131"/>
-      <c r="BK21" s="131"/>
-      <c r="BL21" s="131"/>
+      <c r="I21" s="130"/>
+      <c r="J21" s="130"/>
+      <c r="K21" s="130"/>
+      <c r="L21" s="130"/>
+      <c r="M21" s="130"/>
+      <c r="N21" s="130"/>
+      <c r="O21" s="130"/>
+      <c r="P21" s="130"/>
+      <c r="Q21" s="130"/>
+      <c r="R21" s="130"/>
+      <c r="S21" s="130"/>
+      <c r="T21" s="130"/>
+      <c r="U21" s="130"/>
+      <c r="V21" s="130"/>
+      <c r="W21" s="130"/>
+      <c r="X21" s="130"/>
+      <c r="Y21" s="130"/>
+      <c r="Z21" s="130"/>
+      <c r="AA21" s="130"/>
+      <c r="AB21" s="130"/>
+      <c r="AC21" s="130"/>
+      <c r="AD21" s="130"/>
+      <c r="AE21" s="130"/>
+      <c r="AF21" s="130"/>
+      <c r="AG21" s="130"/>
+      <c r="AH21" s="130"/>
+      <c r="AI21" s="130"/>
+      <c r="AJ21" s="130"/>
+      <c r="AK21" s="130"/>
+      <c r="AL21" s="130"/>
+      <c r="AM21" s="130"/>
+      <c r="AN21" s="130"/>
+      <c r="AO21" s="130"/>
+      <c r="AP21" s="130"/>
+      <c r="AQ21" s="130"/>
+      <c r="AR21" s="130"/>
+      <c r="AS21" s="130"/>
+      <c r="AT21" s="130"/>
+      <c r="AU21" s="130"/>
+      <c r="AV21" s="130"/>
+      <c r="AW21" s="130"/>
+      <c r="AX21" s="130"/>
+      <c r="AY21" s="130"/>
+      <c r="AZ21" s="130"/>
+      <c r="BA21" s="130"/>
+      <c r="BB21" s="130"/>
+      <c r="BC21" s="130"/>
+      <c r="BD21" s="130"/>
+      <c r="BE21" s="130"/>
+      <c r="BF21" s="130"/>
+      <c r="BG21" s="130"/>
+      <c r="BH21" s="130"/>
+      <c r="BI21" s="130"/>
+      <c r="BJ21" s="130"/>
+      <c r="BK21" s="130"/>
+      <c r="BL21" s="130"/>
     </row>
     <row r="22" s="50" customFormat="1" customHeight="1" spans="1:64">
-      <c r="A22" s="51" t="s">
-        <v>33</v>
-      </c>
-      <c r="B22" s="99" t="s">
-        <v>35</v>
-      </c>
-      <c r="C22" s="100"/>
-      <c r="D22" s="101"/>
-      <c r="E22" s="102"/>
-      <c r="F22" s="103"/>
+      <c r="A22" s="51"/>
+      <c r="B22" s="103"/>
+      <c r="C22" s="104"/>
+      <c r="D22" s="105"/>
+      <c r="E22" s="106"/>
+      <c r="F22" s="106"/>
       <c r="G22" s="74"/>
       <c r="H22" s="74" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="I22" s="131"/>
-      <c r="J22" s="131"/>
-      <c r="K22" s="131"/>
-      <c r="L22" s="131"/>
-      <c r="M22" s="131"/>
-      <c r="N22" s="131"/>
-      <c r="O22" s="131"/>
-      <c r="P22" s="131"/>
-      <c r="Q22" s="131"/>
-      <c r="R22" s="131"/>
-      <c r="S22" s="131"/>
-      <c r="T22" s="131"/>
-      <c r="U22" s="131"/>
-      <c r="V22" s="131"/>
-      <c r="W22" s="131"/>
-      <c r="X22" s="131"/>
-      <c r="Y22" s="131"/>
-      <c r="Z22" s="131"/>
-      <c r="AA22" s="131"/>
-      <c r="AB22" s="131"/>
-      <c r="AC22" s="131"/>
-      <c r="AD22" s="131"/>
-      <c r="AE22" s="131"/>
-      <c r="AF22" s="131"/>
-      <c r="AG22" s="131"/>
-      <c r="AH22" s="131"/>
-      <c r="AI22" s="131"/>
-      <c r="AJ22" s="131"/>
-      <c r="AK22" s="131"/>
-      <c r="AL22" s="131"/>
-      <c r="AM22" s="131"/>
-      <c r="AN22" s="131"/>
-      <c r="AO22" s="131"/>
-      <c r="AP22" s="131"/>
-      <c r="AQ22" s="131"/>
-      <c r="AR22" s="131"/>
-      <c r="AS22" s="131"/>
-      <c r="AT22" s="131"/>
-      <c r="AU22" s="131"/>
-      <c r="AV22" s="131"/>
-      <c r="AW22" s="131"/>
-      <c r="AX22" s="131"/>
-      <c r="AY22" s="131"/>
-      <c r="AZ22" s="131"/>
-      <c r="BA22" s="131"/>
-      <c r="BB22" s="131"/>
-      <c r="BC22" s="131"/>
-      <c r="BD22" s="131"/>
-      <c r="BE22" s="131"/>
-      <c r="BF22" s="131"/>
-      <c r="BG22" s="131"/>
-      <c r="BH22" s="131"/>
-      <c r="BI22" s="131"/>
-      <c r="BJ22" s="131"/>
-      <c r="BK22" s="131"/>
-      <c r="BL22" s="131"/>
+      <c r="I22" s="130"/>
+      <c r="J22" s="130"/>
+      <c r="K22" s="130"/>
+      <c r="L22" s="130"/>
+      <c r="M22" s="130"/>
+      <c r="N22" s="130"/>
+      <c r="O22" s="130"/>
+      <c r="P22" s="130"/>
+      <c r="Q22" s="130"/>
+      <c r="R22" s="130"/>
+      <c r="S22" s="130"/>
+      <c r="T22" s="130"/>
+      <c r="U22" s="130"/>
+      <c r="V22" s="130"/>
+      <c r="W22" s="130"/>
+      <c r="X22" s="130"/>
+      <c r="Y22" s="130"/>
+      <c r="Z22" s="130"/>
+      <c r="AA22" s="130"/>
+      <c r="AB22" s="130"/>
+      <c r="AC22" s="130"/>
+      <c r="AD22" s="130"/>
+      <c r="AE22" s="130"/>
+      <c r="AF22" s="130"/>
+      <c r="AG22" s="130"/>
+      <c r="AH22" s="130"/>
+      <c r="AI22" s="130"/>
+      <c r="AJ22" s="130"/>
+      <c r="AK22" s="130"/>
+      <c r="AL22" s="130"/>
+      <c r="AM22" s="130"/>
+      <c r="AN22" s="130"/>
+      <c r="AO22" s="130"/>
+      <c r="AP22" s="130"/>
+      <c r="AQ22" s="130"/>
+      <c r="AR22" s="130"/>
+      <c r="AS22" s="130"/>
+      <c r="AT22" s="130"/>
+      <c r="AU22" s="130"/>
+      <c r="AV22" s="130"/>
+      <c r="AW22" s="130"/>
+      <c r="AX22" s="130"/>
+      <c r="AY22" s="130"/>
+      <c r="AZ22" s="130"/>
+      <c r="BA22" s="130"/>
+      <c r="BB22" s="130"/>
+      <c r="BC22" s="130"/>
+      <c r="BD22" s="130"/>
+      <c r="BE22" s="130"/>
+      <c r="BF22" s="130"/>
+      <c r="BG22" s="130"/>
+      <c r="BH22" s="130"/>
+      <c r="BI22" s="130"/>
+      <c r="BJ22" s="130"/>
+      <c r="BK22" s="130"/>
+      <c r="BL22" s="130"/>
     </row>
     <row r="23" s="50" customFormat="1" customHeight="1" spans="1:64">
       <c r="A23" s="51"/>
-      <c r="B23" s="104"/>
-      <c r="C23" s="105"/>
-      <c r="D23" s="106"/>
-      <c r="E23" s="107"/>
-      <c r="F23" s="107"/>
+      <c r="B23" s="103"/>
+      <c r="C23" s="104"/>
+      <c r="D23" s="105"/>
+      <c r="E23" s="106"/>
+      <c r="F23" s="106"/>
       <c r="G23" s="74"/>
       <c r="H23" s="74" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="I23" s="131"/>
-      <c r="J23" s="131"/>
-      <c r="K23" s="131"/>
-      <c r="L23" s="131"/>
-      <c r="M23" s="131"/>
-      <c r="N23" s="131"/>
-      <c r="O23" s="131"/>
-      <c r="P23" s="131"/>
-      <c r="Q23" s="131"/>
-      <c r="R23" s="131"/>
-      <c r="S23" s="131"/>
-      <c r="T23" s="131"/>
-      <c r="U23" s="131"/>
-      <c r="V23" s="131"/>
-      <c r="W23" s="131"/>
-      <c r="X23" s="131"/>
-      <c r="Y23" s="131"/>
-      <c r="Z23" s="131"/>
-      <c r="AA23" s="131"/>
-      <c r="AB23" s="131"/>
-      <c r="AC23" s="131"/>
-      <c r="AD23" s="131"/>
-      <c r="AE23" s="131"/>
-      <c r="AF23" s="131"/>
-      <c r="AG23" s="131"/>
-      <c r="AH23" s="131"/>
-      <c r="AI23" s="131"/>
-      <c r="AJ23" s="131"/>
-      <c r="AK23" s="131"/>
-      <c r="AL23" s="131"/>
-      <c r="AM23" s="131"/>
-      <c r="AN23" s="131"/>
-      <c r="AO23" s="131"/>
-      <c r="AP23" s="131"/>
-      <c r="AQ23" s="131"/>
-      <c r="AR23" s="131"/>
-      <c r="AS23" s="131"/>
-      <c r="AT23" s="131"/>
-      <c r="AU23" s="131"/>
-      <c r="AV23" s="131"/>
-      <c r="AW23" s="131"/>
-      <c r="AX23" s="131"/>
-      <c r="AY23" s="131"/>
-      <c r="AZ23" s="131"/>
-      <c r="BA23" s="131"/>
-      <c r="BB23" s="131"/>
-      <c r="BC23" s="131"/>
-      <c r="BD23" s="131"/>
-      <c r="BE23" s="131"/>
-      <c r="BF23" s="131"/>
-      <c r="BG23" s="131"/>
-      <c r="BH23" s="131"/>
-      <c r="BI23" s="131"/>
-      <c r="BJ23" s="131"/>
-      <c r="BK23" s="131"/>
-      <c r="BL23" s="131"/>
+      <c r="I23" s="130"/>
+      <c r="J23" s="130"/>
+      <c r="K23" s="130"/>
+      <c r="L23" s="130"/>
+      <c r="M23" s="130"/>
+      <c r="N23" s="130"/>
+      <c r="O23" s="130"/>
+      <c r="P23" s="130"/>
+      <c r="Q23" s="130"/>
+      <c r="R23" s="130"/>
+      <c r="S23" s="130"/>
+      <c r="T23" s="130"/>
+      <c r="U23" s="130"/>
+      <c r="V23" s="130"/>
+      <c r="W23" s="130"/>
+      <c r="X23" s="130"/>
+      <c r="Y23" s="130"/>
+      <c r="Z23" s="130"/>
+      <c r="AA23" s="130"/>
+      <c r="AB23" s="130"/>
+      <c r="AC23" s="130"/>
+      <c r="AD23" s="130"/>
+      <c r="AE23" s="130"/>
+      <c r="AF23" s="130"/>
+      <c r="AG23" s="130"/>
+      <c r="AH23" s="130"/>
+      <c r="AI23" s="130"/>
+      <c r="AJ23" s="130"/>
+      <c r="AK23" s="130"/>
+      <c r="AL23" s="130"/>
+      <c r="AM23" s="130"/>
+      <c r="AN23" s="130"/>
+      <c r="AO23" s="130"/>
+      <c r="AP23" s="130"/>
+      <c r="AQ23" s="130"/>
+      <c r="AR23" s="130"/>
+      <c r="AS23" s="130"/>
+      <c r="AT23" s="130"/>
+      <c r="AU23" s="130"/>
+      <c r="AV23" s="130"/>
+      <c r="AW23" s="130"/>
+      <c r="AX23" s="130"/>
+      <c r="AY23" s="130"/>
+      <c r="AZ23" s="130"/>
+      <c r="BA23" s="130"/>
+      <c r="BB23" s="130"/>
+      <c r="BC23" s="130"/>
+      <c r="BD23" s="130"/>
+      <c r="BE23" s="130"/>
+      <c r="BF23" s="130"/>
+      <c r="BG23" s="130"/>
+      <c r="BH23" s="130"/>
+      <c r="BI23" s="130"/>
+      <c r="BJ23" s="130"/>
+      <c r="BK23" s="130"/>
+      <c r="BL23" s="130"/>
     </row>
     <row r="24" s="50" customFormat="1" customHeight="1" spans="1:64">
       <c r="A24" s="51"/>
-      <c r="B24" s="104"/>
-      <c r="C24" s="105"/>
-      <c r="D24" s="106"/>
-      <c r="E24" s="107"/>
-      <c r="F24" s="107"/>
+      <c r="B24" s="103"/>
+      <c r="C24" s="104"/>
+      <c r="D24" s="105"/>
+      <c r="E24" s="106"/>
+      <c r="F24" s="106"/>
       <c r="G24" s="74"/>
       <c r="H24" s="74" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="I24" s="131"/>
-      <c r="J24" s="131"/>
-      <c r="K24" s="131"/>
-      <c r="L24" s="131"/>
-      <c r="M24" s="131"/>
-      <c r="N24" s="131"/>
-      <c r="O24" s="131"/>
-      <c r="P24" s="131"/>
-      <c r="Q24" s="131"/>
-      <c r="R24" s="131"/>
-      <c r="S24" s="131"/>
-      <c r="T24" s="131"/>
-      <c r="U24" s="131"/>
-      <c r="V24" s="131"/>
-      <c r="W24" s="131"/>
-      <c r="X24" s="131"/>
-      <c r="Y24" s="131"/>
-      <c r="Z24" s="131"/>
-      <c r="AA24" s="131"/>
-      <c r="AB24" s="131"/>
-      <c r="AC24" s="131"/>
-      <c r="AD24" s="131"/>
-      <c r="AE24" s="131"/>
-      <c r="AF24" s="131"/>
-      <c r="AG24" s="131"/>
-      <c r="AH24" s="131"/>
-      <c r="AI24" s="131"/>
-      <c r="AJ24" s="131"/>
-      <c r="AK24" s="131"/>
-      <c r="AL24" s="131"/>
-      <c r="AM24" s="131"/>
-      <c r="AN24" s="131"/>
-      <c r="AO24" s="131"/>
-      <c r="AP24" s="131"/>
-      <c r="AQ24" s="131"/>
-      <c r="AR24" s="131"/>
-      <c r="AS24" s="131"/>
-      <c r="AT24" s="131"/>
-      <c r="AU24" s="131"/>
-      <c r="AV24" s="131"/>
-      <c r="AW24" s="131"/>
-      <c r="AX24" s="131"/>
-      <c r="AY24" s="131"/>
-      <c r="AZ24" s="131"/>
-      <c r="BA24" s="131"/>
-      <c r="BB24" s="131"/>
-      <c r="BC24" s="131"/>
-      <c r="BD24" s="131"/>
-      <c r="BE24" s="131"/>
-      <c r="BF24" s="131"/>
-      <c r="BG24" s="131"/>
-      <c r="BH24" s="131"/>
-      <c r="BI24" s="131"/>
-      <c r="BJ24" s="131"/>
-      <c r="BK24" s="131"/>
-      <c r="BL24" s="131"/>
+      <c r="I24" s="130"/>
+      <c r="J24" s="130"/>
+      <c r="K24" s="130"/>
+      <c r="L24" s="130"/>
+      <c r="M24" s="130"/>
+      <c r="N24" s="130"/>
+      <c r="O24" s="130"/>
+      <c r="P24" s="130"/>
+      <c r="Q24" s="130"/>
+      <c r="R24" s="130"/>
+      <c r="S24" s="130"/>
+      <c r="T24" s="130"/>
+      <c r="U24" s="130"/>
+      <c r="V24" s="130"/>
+      <c r="W24" s="130"/>
+      <c r="X24" s="130"/>
+      <c r="Y24" s="130"/>
+      <c r="Z24" s="130"/>
+      <c r="AA24" s="130"/>
+      <c r="AB24" s="130"/>
+      <c r="AC24" s="130"/>
+      <c r="AD24" s="130"/>
+      <c r="AE24" s="130"/>
+      <c r="AF24" s="130"/>
+      <c r="AG24" s="130"/>
+      <c r="AH24" s="130"/>
+      <c r="AI24" s="130"/>
+      <c r="AJ24" s="130"/>
+      <c r="AK24" s="130"/>
+      <c r="AL24" s="130"/>
+      <c r="AM24" s="130"/>
+      <c r="AN24" s="130"/>
+      <c r="AO24" s="130"/>
+      <c r="AP24" s="130"/>
+      <c r="AQ24" s="130"/>
+      <c r="AR24" s="130"/>
+      <c r="AS24" s="130"/>
+      <c r="AT24" s="130"/>
+      <c r="AU24" s="130"/>
+      <c r="AV24" s="130"/>
+      <c r="AW24" s="130"/>
+      <c r="AX24" s="130"/>
+      <c r="AY24" s="130"/>
+      <c r="AZ24" s="130"/>
+      <c r="BA24" s="130"/>
+      <c r="BB24" s="130"/>
+      <c r="BC24" s="130"/>
+      <c r="BD24" s="130"/>
+      <c r="BE24" s="130"/>
+      <c r="BF24" s="130"/>
+      <c r="BG24" s="130"/>
+      <c r="BH24" s="130"/>
+      <c r="BI24" s="130"/>
+      <c r="BJ24" s="130"/>
+      <c r="BK24" s="130"/>
+      <c r="BL24" s="130"/>
     </row>
     <row r="25" s="50" customFormat="1" customHeight="1" spans="1:64">
       <c r="A25" s="51"/>
-      <c r="B25" s="104"/>
-      <c r="C25" s="105"/>
-      <c r="D25" s="106"/>
-      <c r="E25" s="107"/>
-      <c r="F25" s="107"/>
+      <c r="B25" s="103"/>
+      <c r="C25" s="104"/>
+      <c r="D25" s="105"/>
+      <c r="E25" s="106"/>
+      <c r="F25" s="106"/>
       <c r="G25" s="74"/>
       <c r="H25" s="74" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="I25" s="131"/>
-      <c r="J25" s="131"/>
-      <c r="K25" s="131"/>
-      <c r="L25" s="131"/>
-      <c r="M25" s="131"/>
-      <c r="N25" s="131"/>
-      <c r="O25" s="131"/>
-      <c r="P25" s="131"/>
-      <c r="Q25" s="131"/>
-      <c r="R25" s="131"/>
-      <c r="S25" s="131"/>
-      <c r="T25" s="131"/>
-      <c r="U25" s="131"/>
-      <c r="V25" s="131"/>
-      <c r="W25" s="131"/>
-      <c r="X25" s="131"/>
-      <c r="Y25" s="131"/>
-      <c r="Z25" s="131"/>
-      <c r="AA25" s="131"/>
-      <c r="AB25" s="131"/>
-      <c r="AC25" s="131"/>
-      <c r="AD25" s="131"/>
-      <c r="AE25" s="131"/>
-      <c r="AF25" s="131"/>
-      <c r="AG25" s="131"/>
-      <c r="AH25" s="131"/>
-      <c r="AI25" s="131"/>
-      <c r="AJ25" s="131"/>
-      <c r="AK25" s="131"/>
-      <c r="AL25" s="131"/>
-      <c r="AM25" s="131"/>
-      <c r="AN25" s="131"/>
-      <c r="AO25" s="131"/>
-      <c r="AP25" s="131"/>
-      <c r="AQ25" s="131"/>
-      <c r="AR25" s="131"/>
-      <c r="AS25" s="131"/>
-      <c r="AT25" s="131"/>
-      <c r="AU25" s="131"/>
-      <c r="AV25" s="131"/>
-      <c r="AW25" s="131"/>
-      <c r="AX25" s="131"/>
-      <c r="AY25" s="131"/>
-      <c r="AZ25" s="131"/>
-      <c r="BA25" s="131"/>
-      <c r="BB25" s="131"/>
-      <c r="BC25" s="131"/>
-      <c r="BD25" s="131"/>
-      <c r="BE25" s="131"/>
-      <c r="BF25" s="131"/>
-      <c r="BG25" s="131"/>
-      <c r="BH25" s="131"/>
-      <c r="BI25" s="131"/>
-      <c r="BJ25" s="131"/>
-      <c r="BK25" s="131"/>
-      <c r="BL25" s="131"/>
+      <c r="I25" s="130"/>
+      <c r="J25" s="130"/>
+      <c r="K25" s="130"/>
+      <c r="L25" s="130"/>
+      <c r="M25" s="130"/>
+      <c r="N25" s="130"/>
+      <c r="O25" s="130"/>
+      <c r="P25" s="130"/>
+      <c r="Q25" s="130"/>
+      <c r="R25" s="130"/>
+      <c r="S25" s="130"/>
+      <c r="T25" s="130"/>
+      <c r="U25" s="130"/>
+      <c r="V25" s="130"/>
+      <c r="W25" s="130"/>
+      <c r="X25" s="130"/>
+      <c r="Y25" s="130"/>
+      <c r="Z25" s="130"/>
+      <c r="AA25" s="130"/>
+      <c r="AB25" s="130"/>
+      <c r="AC25" s="130"/>
+      <c r="AD25" s="130"/>
+      <c r="AE25" s="130"/>
+      <c r="AF25" s="130"/>
+      <c r="AG25" s="130"/>
+      <c r="AH25" s="130"/>
+      <c r="AI25" s="130"/>
+      <c r="AJ25" s="130"/>
+      <c r="AK25" s="130"/>
+      <c r="AL25" s="130"/>
+      <c r="AM25" s="130"/>
+      <c r="AN25" s="130"/>
+      <c r="AO25" s="130"/>
+      <c r="AP25" s="130"/>
+      <c r="AQ25" s="130"/>
+      <c r="AR25" s="130"/>
+      <c r="AS25" s="130"/>
+      <c r="AT25" s="130"/>
+      <c r="AU25" s="130"/>
+      <c r="AV25" s="130"/>
+      <c r="AW25" s="130"/>
+      <c r="AX25" s="130"/>
+      <c r="AY25" s="130"/>
+      <c r="AZ25" s="130"/>
+      <c r="BA25" s="130"/>
+      <c r="BB25" s="130"/>
+      <c r="BC25" s="130"/>
+      <c r="BD25" s="130"/>
+      <c r="BE25" s="130"/>
+      <c r="BF25" s="130"/>
+      <c r="BG25" s="130"/>
+      <c r="BH25" s="130"/>
+      <c r="BI25" s="130"/>
+      <c r="BJ25" s="130"/>
+      <c r="BK25" s="130"/>
+      <c r="BL25" s="130"/>
     </row>
     <row r="26" s="50" customFormat="1" customHeight="1" spans="1:64">
       <c r="A26" s="51"/>
-      <c r="B26" s="104"/>
-      <c r="C26" s="105"/>
-      <c r="D26" s="106"/>
-      <c r="E26" s="107"/>
-      <c r="F26" s="107"/>
+      <c r="B26" s="103"/>
+      <c r="C26" s="104"/>
+      <c r="D26" s="105"/>
+      <c r="E26" s="106"/>
+      <c r="F26" s="106"/>
       <c r="G26" s="74"/>
       <c r="H26" s="74" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="I26" s="131"/>
-      <c r="J26" s="131"/>
-      <c r="K26" s="131"/>
-      <c r="L26" s="131"/>
-      <c r="M26" s="131"/>
-      <c r="N26" s="131"/>
-      <c r="O26" s="131"/>
-      <c r="P26" s="131"/>
-      <c r="Q26" s="131"/>
-      <c r="R26" s="131"/>
-      <c r="S26" s="131"/>
-      <c r="T26" s="131"/>
-      <c r="U26" s="131"/>
-      <c r="V26" s="131"/>
-      <c r="W26" s="131"/>
-      <c r="X26" s="131"/>
-      <c r="Y26" s="131"/>
-      <c r="Z26" s="131"/>
-      <c r="AA26" s="131"/>
-      <c r="AB26" s="131"/>
-      <c r="AC26" s="131"/>
-      <c r="AD26" s="131"/>
-      <c r="AE26" s="131"/>
-      <c r="AF26" s="131"/>
-      <c r="AG26" s="131"/>
-      <c r="AH26" s="131"/>
-      <c r="AI26" s="131"/>
-      <c r="AJ26" s="131"/>
-      <c r="AK26" s="131"/>
-      <c r="AL26" s="131"/>
-      <c r="AM26" s="131"/>
-      <c r="AN26" s="131"/>
-      <c r="AO26" s="131"/>
-      <c r="AP26" s="131"/>
-      <c r="AQ26" s="131"/>
-      <c r="AR26" s="131"/>
-      <c r="AS26" s="131"/>
-      <c r="AT26" s="131"/>
-      <c r="AU26" s="131"/>
-      <c r="AV26" s="131"/>
-      <c r="AW26" s="131"/>
-      <c r="AX26" s="131"/>
-      <c r="AY26" s="131"/>
-      <c r="AZ26" s="131"/>
-      <c r="BA26" s="131"/>
-      <c r="BB26" s="131"/>
-      <c r="BC26" s="131"/>
-      <c r="BD26" s="131"/>
-      <c r="BE26" s="131"/>
-      <c r="BF26" s="131"/>
-      <c r="BG26" s="131"/>
-      <c r="BH26" s="131"/>
-      <c r="BI26" s="131"/>
-      <c r="BJ26" s="131"/>
-      <c r="BK26" s="131"/>
-      <c r="BL26" s="131"/>
+      <c r="I26" s="130"/>
+      <c r="J26" s="130"/>
+      <c r="K26" s="130"/>
+      <c r="L26" s="130"/>
+      <c r="M26" s="130"/>
+      <c r="N26" s="130"/>
+      <c r="O26" s="130"/>
+      <c r="P26" s="130"/>
+      <c r="Q26" s="130"/>
+      <c r="R26" s="130"/>
+      <c r="S26" s="130"/>
+      <c r="T26" s="130"/>
+      <c r="U26" s="130"/>
+      <c r="V26" s="130"/>
+      <c r="W26" s="130"/>
+      <c r="X26" s="130"/>
+      <c r="Y26" s="130"/>
+      <c r="Z26" s="130"/>
+      <c r="AA26" s="130"/>
+      <c r="AB26" s="130"/>
+      <c r="AC26" s="130"/>
+      <c r="AD26" s="130"/>
+      <c r="AE26" s="130"/>
+      <c r="AF26" s="130"/>
+      <c r="AG26" s="130"/>
+      <c r="AH26" s="130"/>
+      <c r="AI26" s="130"/>
+      <c r="AJ26" s="130"/>
+      <c r="AK26" s="130"/>
+      <c r="AL26" s="130"/>
+      <c r="AM26" s="130"/>
+      <c r="AN26" s="130"/>
+      <c r="AO26" s="130"/>
+      <c r="AP26" s="130"/>
+      <c r="AQ26" s="130"/>
+      <c r="AR26" s="130"/>
+      <c r="AS26" s="130"/>
+      <c r="AT26" s="130"/>
+      <c r="AU26" s="130"/>
+      <c r="AV26" s="130"/>
+      <c r="AW26" s="130"/>
+      <c r="AX26" s="130"/>
+      <c r="AY26" s="130"/>
+      <c r="AZ26" s="130"/>
+      <c r="BA26" s="130"/>
+      <c r="BB26" s="130"/>
+      <c r="BC26" s="130"/>
+      <c r="BD26" s="130"/>
+      <c r="BE26" s="130"/>
+      <c r="BF26" s="130"/>
+      <c r="BG26" s="130"/>
+      <c r="BH26" s="130"/>
+      <c r="BI26" s="130"/>
+      <c r="BJ26" s="130"/>
+      <c r="BK26" s="130"/>
+      <c r="BL26" s="130"/>
     </row>
     <row r="27" s="50" customFormat="1" customHeight="1" spans="1:64">
-      <c r="A27" s="51"/>
-      <c r="B27" s="104"/>
-      <c r="C27" s="105"/>
-      <c r="D27" s="106"/>
-      <c r="E27" s="107"/>
-      <c r="F27" s="107"/>
+      <c r="A27" s="51" t="s">
+        <v>38</v>
+      </c>
+      <c r="B27" s="107"/>
+      <c r="C27" s="108"/>
+      <c r="D27" s="109"/>
+      <c r="E27" s="110"/>
+      <c r="F27" s="110"/>
       <c r="G27" s="74"/>
       <c r="H27" s="74" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="I27" s="131"/>
-      <c r="J27" s="131"/>
-      <c r="K27" s="131"/>
-      <c r="L27" s="131"/>
-      <c r="M27" s="131"/>
-      <c r="N27" s="131"/>
-      <c r="O27" s="131"/>
-      <c r="P27" s="131"/>
-      <c r="Q27" s="131"/>
-      <c r="R27" s="131"/>
-      <c r="S27" s="131"/>
-      <c r="T27" s="131"/>
-      <c r="U27" s="131"/>
-      <c r="V27" s="131"/>
-      <c r="W27" s="131"/>
-      <c r="X27" s="131"/>
-      <c r="Y27" s="131"/>
-      <c r="Z27" s="131"/>
-      <c r="AA27" s="131"/>
-      <c r="AB27" s="131"/>
-      <c r="AC27" s="131"/>
-      <c r="AD27" s="131"/>
-      <c r="AE27" s="131"/>
-      <c r="AF27" s="131"/>
-      <c r="AG27" s="131"/>
-      <c r="AH27" s="131"/>
-      <c r="AI27" s="131"/>
-      <c r="AJ27" s="131"/>
-      <c r="AK27" s="131"/>
-      <c r="AL27" s="131"/>
-      <c r="AM27" s="131"/>
-      <c r="AN27" s="131"/>
-      <c r="AO27" s="131"/>
-      <c r="AP27" s="131"/>
-      <c r="AQ27" s="131"/>
-      <c r="AR27" s="131"/>
-      <c r="AS27" s="131"/>
-      <c r="AT27" s="131"/>
-      <c r="AU27" s="131"/>
-      <c r="AV27" s="131"/>
-      <c r="AW27" s="131"/>
-      <c r="AX27" s="131"/>
-      <c r="AY27" s="131"/>
-      <c r="AZ27" s="131"/>
-      <c r="BA27" s="131"/>
-      <c r="BB27" s="131"/>
-      <c r="BC27" s="131"/>
-      <c r="BD27" s="131"/>
-      <c r="BE27" s="131"/>
-      <c r="BF27" s="131"/>
-      <c r="BG27" s="131"/>
-      <c r="BH27" s="131"/>
-      <c r="BI27" s="131"/>
-      <c r="BJ27" s="131"/>
-      <c r="BK27" s="131"/>
-      <c r="BL27" s="131"/>
+      <c r="I27" s="130"/>
+      <c r="J27" s="130"/>
+      <c r="K27" s="130"/>
+      <c r="L27" s="130"/>
+      <c r="M27" s="130"/>
+      <c r="N27" s="130"/>
+      <c r="O27" s="130"/>
+      <c r="P27" s="130"/>
+      <c r="Q27" s="130"/>
+      <c r="R27" s="130"/>
+      <c r="S27" s="130"/>
+      <c r="T27" s="130"/>
+      <c r="U27" s="130"/>
+      <c r="V27" s="130"/>
+      <c r="W27" s="130"/>
+      <c r="X27" s="130"/>
+      <c r="Y27" s="130"/>
+      <c r="Z27" s="130"/>
+      <c r="AA27" s="130"/>
+      <c r="AB27" s="130"/>
+      <c r="AC27" s="130"/>
+      <c r="AD27" s="130"/>
+      <c r="AE27" s="130"/>
+      <c r="AF27" s="130"/>
+      <c r="AG27" s="130"/>
+      <c r="AH27" s="130"/>
+      <c r="AI27" s="130"/>
+      <c r="AJ27" s="130"/>
+      <c r="AK27" s="130"/>
+      <c r="AL27" s="130"/>
+      <c r="AM27" s="130"/>
+      <c r="AN27" s="130"/>
+      <c r="AO27" s="130"/>
+      <c r="AP27" s="130"/>
+      <c r="AQ27" s="130"/>
+      <c r="AR27" s="130"/>
+      <c r="AS27" s="130"/>
+      <c r="AT27" s="130"/>
+      <c r="AU27" s="130"/>
+      <c r="AV27" s="130"/>
+      <c r="AW27" s="130"/>
+      <c r="AX27" s="130"/>
+      <c r="AY27" s="130"/>
+      <c r="AZ27" s="130"/>
+      <c r="BA27" s="130"/>
+      <c r="BB27" s="130"/>
+      <c r="BC27" s="130"/>
+      <c r="BD27" s="130"/>
+      <c r="BE27" s="130"/>
+      <c r="BF27" s="130"/>
+      <c r="BG27" s="130"/>
+      <c r="BH27" s="130"/>
+      <c r="BI27" s="130"/>
+      <c r="BJ27" s="130"/>
+      <c r="BK27" s="130"/>
+      <c r="BL27" s="130"/>
     </row>
     <row r="28" s="50" customFormat="1" customHeight="1" spans="1:64">
-      <c r="A28" s="51" t="s">
-        <v>36</v>
-      </c>
-      <c r="B28" s="108"/>
-      <c r="C28" s="109"/>
-      <c r="D28" s="110"/>
-      <c r="E28" s="111"/>
-      <c r="F28" s="111"/>
-      <c r="G28" s="74"/>
-      <c r="H28" s="74" t="str">
+      <c r="A28" s="52" t="s">
+        <v>39</v>
+      </c>
+      <c r="B28" s="111" t="s">
+        <v>40</v>
+      </c>
+      <c r="C28" s="112"/>
+      <c r="D28" s="113"/>
+      <c r="E28" s="114"/>
+      <c r="F28" s="115"/>
+      <c r="G28" s="116"/>
+      <c r="H28" s="116" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
@@ -4585,88 +4623,15 @@
       <c r="BK28" s="131"/>
       <c r="BL28" s="131"/>
     </row>
-    <row r="29" s="50" customFormat="1" customHeight="1" spans="1:64">
-      <c r="A29" s="52" t="s">
-        <v>37</v>
-      </c>
-      <c r="B29" s="112" t="s">
-        <v>38</v>
-      </c>
-      <c r="C29" s="113"/>
-      <c r="D29" s="114"/>
-      <c r="E29" s="115"/>
-      <c r="F29" s="116"/>
+    <row r="29" customHeight="1" spans="7:7">
       <c r="G29" s="117"/>
-      <c r="H29" s="117" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="I29" s="132"/>
-      <c r="J29" s="132"/>
-      <c r="K29" s="132"/>
-      <c r="L29" s="132"/>
-      <c r="M29" s="132"/>
-      <c r="N29" s="132"/>
-      <c r="O29" s="132"/>
-      <c r="P29" s="132"/>
-      <c r="Q29" s="132"/>
-      <c r="R29" s="132"/>
-      <c r="S29" s="132"/>
-      <c r="T29" s="132"/>
-      <c r="U29" s="132"/>
-      <c r="V29" s="132"/>
-      <c r="W29" s="132"/>
-      <c r="X29" s="132"/>
-      <c r="Y29" s="132"/>
-      <c r="Z29" s="132"/>
-      <c r="AA29" s="132"/>
-      <c r="AB29" s="132"/>
-      <c r="AC29" s="132"/>
-      <c r="AD29" s="132"/>
-      <c r="AE29" s="132"/>
-      <c r="AF29" s="132"/>
-      <c r="AG29" s="132"/>
-      <c r="AH29" s="132"/>
-      <c r="AI29" s="132"/>
-      <c r="AJ29" s="132"/>
-      <c r="AK29" s="132"/>
-      <c r="AL29" s="132"/>
-      <c r="AM29" s="132"/>
-      <c r="AN29" s="132"/>
-      <c r="AO29" s="132"/>
-      <c r="AP29" s="132"/>
-      <c r="AQ29" s="132"/>
-      <c r="AR29" s="132"/>
-      <c r="AS29" s="132"/>
-      <c r="AT29" s="132"/>
-      <c r="AU29" s="132"/>
-      <c r="AV29" s="132"/>
-      <c r="AW29" s="132"/>
-      <c r="AX29" s="132"/>
-      <c r="AY29" s="132"/>
-      <c r="AZ29" s="132"/>
-      <c r="BA29" s="132"/>
-      <c r="BB29" s="132"/>
-      <c r="BC29" s="132"/>
-      <c r="BD29" s="132"/>
-      <c r="BE29" s="132"/>
-      <c r="BF29" s="132"/>
-      <c r="BG29" s="132"/>
-      <c r="BH29" s="132"/>
-      <c r="BI29" s="132"/>
-      <c r="BJ29" s="132"/>
-      <c r="BK29" s="132"/>
-      <c r="BL29" s="132"/>
-    </row>
-    <row r="30" customHeight="1" spans="7:7">
-      <c r="G30" s="118"/>
-    </row>
-    <row r="31" customHeight="1" spans="3:6">
-      <c r="C31" s="119"/>
-      <c r="F31" s="120"/>
-    </row>
-    <row r="32" customHeight="1" spans="3:3">
-      <c r="C32" s="121"/>
+    </row>
+    <row r="30" customHeight="1" spans="3:6">
+      <c r="C30" s="118"/>
+      <c r="F30" s="119"/>
+    </row>
+    <row r="31" customHeight="1" spans="3:3">
+      <c r="C31" s="120"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -4682,7 +4647,7 @@
     <mergeCell ref="BF4:BL4"/>
     <mergeCell ref="C5:D5"/>
   </mergeCells>
-  <conditionalFormatting sqref="D7:D29">
+  <conditionalFormatting sqref="D7:D28">
     <cfRule type="dataBar" priority="14">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -4691,17 +4656,17 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{a99c5aa5-d06a-4570-bd23-d23678131646}</x14:id>
+          <x14:id>{9dc4eb3f-637f-49d5-b57d-922f6ef5b741}</x14:id>
         </ext>
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I5:BL29">
+  <conditionalFormatting sqref="I5:BL28">
     <cfRule type="expression" dxfId="0" priority="33">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I7:BL29">
+  <conditionalFormatting sqref="I7:BL28">
     <cfRule type="expression" dxfId="1" priority="27">
       <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
     </cfRule>
@@ -4728,7 +4693,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{a99c5aa5-d06a-4570-bd23-d23678131646}">
+          <x14:cfRule type="dataBar" id="{9dc4eb3f-637f-49d5-b57d-922f6ef5b741}">
             <x14:dataBar minLength="0" maxLength="100" gradient="0">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -4740,7 +4705,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D7:D29</xm:sqref>
+          <xm:sqref>D7:D28</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -4753,10 +4718,10 @@
   <sheetPr/>
   <dimension ref="A1:Q27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
       <selection/>
-      <selection pane="topRight" activeCell="Q9" sqref="Q9"/>
+      <selection pane="topRight" activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
@@ -4776,13 +4741,13 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" ht="54" customHeight="1" spans="1:17">
       <c r="A1" s="3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="5"/>
       <c r="D1" s="6"/>
       <c r="E1" s="7" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="F1" s="8"/>
       <c r="G1" s="8"/>
@@ -4792,7 +4757,7 @@
         <v>1</v>
       </c>
       <c r="L1" s="7" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="M1" s="8"/>
       <c r="N1" s="8"/>
@@ -4805,54 +4770,54 @@
     <row r="2" s="1" customFormat="1" ht="21" customHeight="1" spans="1:17">
       <c r="A2" s="9"/>
       <c r="B2" s="10" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="12"/>
       <c r="F2" s="13" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="G2" s="14" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="H2" s="14" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="I2" s="14" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="J2" s="46" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="L2" s="12"/>
       <c r="M2" s="13" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="N2" s="14" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="O2" s="14" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="P2" s="14" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="Q2" s="46" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:17">
       <c r="A3" s="15" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B3" s="16"/>
       <c r="C3" s="17"/>
       <c r="D3" s="18"/>
       <c r="E3" s="15" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="F3" s="16"/>
       <c r="G3" s="19"/>
@@ -4860,7 +4825,7 @@
       <c r="I3" s="19"/>
       <c r="J3" s="17"/>
       <c r="L3" s="15" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="M3" s="16"/>
       <c r="N3" s="19"/>
@@ -4874,13 +4839,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="22" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D4" s="18"/>
       <c r="E4" s="23"/>
       <c r="F4" s="24"/>
       <c r="G4" s="24" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="H4" s="25">
         <f>J1+0.1</f>
@@ -4897,7 +4862,7 @@
       <c r="L4" s="23"/>
       <c r="M4" s="24"/>
       <c r="N4" s="24" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="O4" s="25">
         <f>Q1+0.1</f>
@@ -4918,7 +4883,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="22" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D5" s="18"/>
       <c r="E5" s="26"/>
@@ -4926,39 +4891,39 @@
         <v>1</v>
       </c>
       <c r="G5" s="28" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="H5" s="29" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="I5" s="29" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="J5" s="48" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="L5" s="26"/>
       <c r="M5" s="27">
         <v>1</v>
       </c>
       <c r="N5" s="28" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="O5" s="29" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="P5" s="29" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="Q5" s="48" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:17">
       <c r="A6" s="20"/>
       <c r="B6" s="21"/>
       <c r="C6" s="30" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D6" s="18"/>
       <c r="E6" s="26"/>
@@ -4974,21 +4939,23 @@
         <v>2</v>
       </c>
       <c r="N6" s="28" t="s">
-        <v>53</v>
-      </c>
-      <c r="O6" s="29"/>
-      <c r="P6" s="29">
-        <v>1.21</v>
+        <v>31</v>
+      </c>
+      <c r="O6" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="P6" s="29" t="s">
+        <v>52</v>
       </c>
       <c r="Q6" s="48" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:17">
       <c r="A7" s="20"/>
       <c r="B7" s="21"/>
       <c r="C7" s="30" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D7" s="18"/>
       <c r="E7" s="26"/>
@@ -4996,24 +4963,26 @@
         <v>3</v>
       </c>
       <c r="G7" s="28" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H7" s="29"/>
       <c r="I7" s="29"/>
-      <c r="J7" s="48">
-        <v>1.31</v>
-      </c>
+      <c r="J7" s="48"/>
       <c r="L7" s="26"/>
       <c r="M7" s="27">
         <v>3</v>
       </c>
       <c r="N7" s="28" t="s">
-        <v>56</v>
-      </c>
-      <c r="O7" s="29"/>
-      <c r="P7" s="29"/>
-      <c r="Q7" s="48">
-        <v>2.31</v>
+        <v>35</v>
+      </c>
+      <c r="O7" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="P7" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q7" s="48" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="8" ht="15.15" spans="1:17">
@@ -5036,25 +5005,29 @@
         <v>4</v>
       </c>
       <c r="N8" s="33" t="s">
-        <v>58</v>
-      </c>
-      <c r="O8" s="34"/>
-      <c r="P8" s="34"/>
+        <v>36</v>
+      </c>
+      <c r="O8" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="P8" s="34" t="s">
+        <v>52</v>
+      </c>
       <c r="Q8" s="49">
-        <v>2.32</v>
+        <v>2.31</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="20"/>
       <c r="B9" s="21"/>
       <c r="C9" s="30" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D9" s="18"/>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="35" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B10" s="36"/>
       <c r="C10" s="37"/>
@@ -5066,7 +5039,7 @@
         <v>1</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D11" s="18"/>
     </row>
@@ -5076,13 +5049,13 @@
         <v>2</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D12" s="18"/>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="38" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B13" s="39"/>
       <c r="C13" s="40"/>
@@ -5094,7 +5067,7 @@
         <v>1</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D14" s="18"/>
     </row>
@@ -5104,7 +5077,7 @@
         <v>2</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D15" s="18"/>
     </row>
@@ -5114,7 +5087,7 @@
         <v>3</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D16" s="18"/>
     </row>
@@ -5124,7 +5097,7 @@
         <v>4</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D17" s="18"/>
     </row>
@@ -5134,7 +5107,7 @@
         <v>5</v>
       </c>
       <c r="C18" s="30" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D18" s="18"/>
     </row>
@@ -5144,7 +5117,7 @@
         <v>6</v>
       </c>
       <c r="C19" s="43" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D19" s="18"/>
     </row>

</xml_diff>